<commit_message>
seatgen done, db made, need to do invigilation
</commit_message>
<xml_diff>
--- a/BE/Aarrangement.xlsx
+++ b/BE/Aarrangement.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E393"/>
+  <dimension ref="A1:D393"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,9 +415,6 @@
       <c r="D1" t="str">
         <v>SEAT</v>
       </c>
-      <c r="E1" t="str">
-        <v>INVIGILATOR</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -432,9 +429,6 @@
       <c r="D2" t="str">
         <v>1A</v>
       </c>
-      <c r="E2" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -449,9 +443,6 @@
       <c r="D3" t="str">
         <v>1C</v>
       </c>
-      <c r="E3" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -466,9 +457,6 @@
       <c r="D4" t="str">
         <v>1E</v>
       </c>
-      <c r="E4" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -483,9 +471,6 @@
       <c r="D5" t="str">
         <v>1G</v>
       </c>
-      <c r="E5" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -500,9 +485,6 @@
       <c r="D6" t="str">
         <v>1I</v>
       </c>
-      <c r="E6" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -516,9 +498,6 @@
       </c>
       <c r="D7" t="str">
         <v>2B</v>
-      </c>
-      <c r="E7" t="str">
-        <v>horseman</v>
       </c>
     </row>
     <row r="8">
@@ -534,9 +513,6 @@
       <c r="D8" t="str">
         <v>2D</v>
       </c>
-      <c r="E8" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -551,9 +527,6 @@
       <c r="D9" t="str">
         <v>2F</v>
       </c>
-      <c r="E9" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -568,9 +541,6 @@
       <c r="D10" t="str">
         <v>2H</v>
       </c>
-      <c r="E10" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -585,9 +555,6 @@
       <c r="D11" t="str">
         <v>2J</v>
       </c>
-      <c r="E11" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -602,9 +569,6 @@
       <c r="D12" t="str">
         <v>3C</v>
       </c>
-      <c r="E12" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -619,9 +583,6 @@
       <c r="D13" t="str">
         <v>3E</v>
       </c>
-      <c r="E13" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -636,9 +597,6 @@
       <c r="D14" t="str">
         <v>3G</v>
       </c>
-      <c r="E14" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -653,9 +611,6 @@
       <c r="D15" t="str">
         <v>3I</v>
       </c>
-      <c r="E15" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -670,9 +625,6 @@
       <c r="D16" t="str">
         <v>4A</v>
       </c>
-      <c r="E16" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -687,9 +639,6 @@
       <c r="D17" t="str">
         <v>4C</v>
       </c>
-      <c r="E17" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -704,9 +653,6 @@
       <c r="D18" t="str">
         <v>4E</v>
       </c>
-      <c r="E18" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -721,9 +667,6 @@
       <c r="D19" t="str">
         <v>4G</v>
       </c>
-      <c r="E19" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -738,9 +681,6 @@
       <c r="D20" t="str">
         <v>4I</v>
       </c>
-      <c r="E20" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -755,9 +695,6 @@
       <c r="D21" t="str">
         <v>5B</v>
       </c>
-      <c r="E21" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -772,9 +709,6 @@
       <c r="D22" t="str">
         <v>5D</v>
       </c>
-      <c r="E22" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -789,9 +723,6 @@
       <c r="D23" t="str">
         <v>5F</v>
       </c>
-      <c r="E23" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -806,9 +737,6 @@
       <c r="D24" t="str">
         <v>5H</v>
       </c>
-      <c r="E24" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -823,9 +751,6 @@
       <c r="D25" t="str">
         <v>5J</v>
       </c>
-      <c r="E25" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -840,9 +765,6 @@
       <c r="D26" t="str">
         <v>6C</v>
       </c>
-      <c r="E26" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -857,9 +779,6 @@
       <c r="D27" t="str">
         <v>6E</v>
       </c>
-      <c r="E27" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -874,9 +793,6 @@
       <c r="D28" t="str">
         <v>6G</v>
       </c>
-      <c r="E28" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -891,9 +807,6 @@
       <c r="D29" t="str">
         <v>6I</v>
       </c>
-      <c r="E29" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -908,9 +821,6 @@
       <c r="D30" t="str">
         <v>7A</v>
       </c>
-      <c r="E30" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -925,9 +835,6 @@
       <c r="D31" t="str">
         <v>7C</v>
       </c>
-      <c r="E31" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -942,9 +849,6 @@
       <c r="D32" t="str">
         <v>7E</v>
       </c>
-      <c r="E32" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -959,9 +863,6 @@
       <c r="D33" t="str">
         <v>7G</v>
       </c>
-      <c r="E33" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -976,9 +877,6 @@
       <c r="D34" t="str">
         <v>7I</v>
       </c>
-      <c r="E34" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -993,9 +891,6 @@
       <c r="D35" t="str">
         <v>8B</v>
       </c>
-      <c r="E35" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -1010,9 +905,6 @@
       <c r="D36" t="str">
         <v>8D</v>
       </c>
-      <c r="E36" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -1027,9 +919,6 @@
       <c r="D37" t="str">
         <v>8F</v>
       </c>
-      <c r="E37" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -1044,9 +933,6 @@
       <c r="D38" t="str">
         <v>8H</v>
       </c>
-      <c r="E38" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -1061,9 +947,6 @@
       <c r="D39" t="str">
         <v>8J</v>
       </c>
-      <c r="E39" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -1078,9 +961,6 @@
       <c r="D40" t="str">
         <v>9C</v>
       </c>
-      <c r="E40" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -1095,9 +975,6 @@
       <c r="D41" t="str">
         <v>9E</v>
       </c>
-      <c r="E41" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -1112,9 +989,6 @@
       <c r="D42" t="str">
         <v>9G</v>
       </c>
-      <c r="E42" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -1129,9 +1003,6 @@
       <c r="D43" t="str">
         <v>9I</v>
       </c>
-      <c r="E43" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -1146,9 +1017,6 @@
       <c r="D44" t="str">
         <v>10A</v>
       </c>
-      <c r="E44" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -1163,9 +1031,6 @@
       <c r="D45" t="str">
         <v>10C</v>
       </c>
-      <c r="E45" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -1180,9 +1045,6 @@
       <c r="D46" t="str">
         <v>10E</v>
       </c>
-      <c r="E46" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -1197,9 +1059,6 @@
       <c r="D47" t="str">
         <v>10G</v>
       </c>
-      <c r="E47" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -1214,9 +1073,6 @@
       <c r="D48" t="str">
         <v>10I</v>
       </c>
-      <c r="E48" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -1231,9 +1087,6 @@
       <c r="D49" t="str">
         <v>1A</v>
       </c>
-      <c r="E49" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -1248,9 +1101,6 @@
       <c r="D50" t="str">
         <v>1C</v>
       </c>
-      <c r="E50" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -1265,9 +1115,6 @@
       <c r="D51" t="str">
         <v>1E</v>
       </c>
-      <c r="E51" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -1282,9 +1129,6 @@
       <c r="D52" t="str">
         <v>1G</v>
       </c>
-      <c r="E52" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -1299,9 +1143,6 @@
       <c r="D53" t="str">
         <v>1I</v>
       </c>
-      <c r="E53" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -1316,9 +1157,6 @@
       <c r="D54" t="str">
         <v>1K</v>
       </c>
-      <c r="E54" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -1333,9 +1171,6 @@
       <c r="D55" t="str">
         <v>2B</v>
       </c>
-      <c r="E55" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -1350,9 +1185,6 @@
       <c r="D56" t="str">
         <v>2D</v>
       </c>
-      <c r="E56" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -1367,9 +1199,6 @@
       <c r="D57" t="str">
         <v>2F</v>
       </c>
-      <c r="E57" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -1384,9 +1213,6 @@
       <c r="D58" t="str">
         <v>2H</v>
       </c>
-      <c r="E58" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -1401,9 +1227,6 @@
       <c r="D59" t="str">
         <v>2J</v>
       </c>
-      <c r="E59" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -1418,9 +1241,6 @@
       <c r="D60" t="str">
         <v>3C</v>
       </c>
-      <c r="E60" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -1435,9 +1255,6 @@
       <c r="D61" t="str">
         <v>3E</v>
       </c>
-      <c r="E61" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -1452,9 +1269,6 @@
       <c r="D62" t="str">
         <v>3G</v>
       </c>
-      <c r="E62" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -1469,9 +1283,6 @@
       <c r="D63" t="str">
         <v>3I</v>
       </c>
-      <c r="E63" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -1486,9 +1297,6 @@
       <c r="D64" t="str">
         <v>3K</v>
       </c>
-      <c r="E64" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -1503,9 +1311,6 @@
       <c r="D65" t="str">
         <v>4A</v>
       </c>
-      <c r="E65" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -1520,9 +1325,6 @@
       <c r="D66" t="str">
         <v>4C</v>
       </c>
-      <c r="E66" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -1537,9 +1339,6 @@
       <c r="D67" t="str">
         <v>4E</v>
       </c>
-      <c r="E67" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -1554,9 +1353,6 @@
       <c r="D68" t="str">
         <v>4G</v>
       </c>
-      <c r="E68" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -1571,9 +1367,6 @@
       <c r="D69" t="str">
         <v>4I</v>
       </c>
-      <c r="E69" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -1588,9 +1381,6 @@
       <c r="D70" t="str">
         <v>4K</v>
       </c>
-      <c r="E70" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -1605,9 +1395,6 @@
       <c r="D71" t="str">
         <v>5B</v>
       </c>
-      <c r="E71" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -1622,9 +1409,6 @@
       <c r="D72" t="str">
         <v>5D</v>
       </c>
-      <c r="E72" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -1639,9 +1423,6 @@
       <c r="D73" t="str">
         <v>5F</v>
       </c>
-      <c r="E73" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -1656,9 +1437,6 @@
       <c r="D74" t="str">
         <v>5H</v>
       </c>
-      <c r="E74" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -1673,9 +1451,6 @@
       <c r="D75" t="str">
         <v>5J</v>
       </c>
-      <c r="E75" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -1690,9 +1465,6 @@
       <c r="D76" t="str">
         <v>6C</v>
       </c>
-      <c r="E76" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -1707,9 +1479,6 @@
       <c r="D77" t="str">
         <v>6E</v>
       </c>
-      <c r="E77" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -1724,9 +1493,6 @@
       <c r="D78" t="str">
         <v>6G</v>
       </c>
-      <c r="E78" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -1741,9 +1507,6 @@
       <c r="D79" t="str">
         <v>6I</v>
       </c>
-      <c r="E79" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -1758,9 +1521,6 @@
       <c r="D80" t="str">
         <v>6K</v>
       </c>
-      <c r="E80" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -1775,9 +1535,6 @@
       <c r="D81" t="str">
         <v>7A</v>
       </c>
-      <c r="E81" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -1792,9 +1549,6 @@
       <c r="D82" t="str">
         <v>7C</v>
       </c>
-      <c r="E82" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -1809,9 +1563,6 @@
       <c r="D83" t="str">
         <v>7E</v>
       </c>
-      <c r="E83" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -1826,9 +1577,6 @@
       <c r="D84" t="str">
         <v>7G</v>
       </c>
-      <c r="E84" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -1843,9 +1591,6 @@
       <c r="D85" t="str">
         <v>7I</v>
       </c>
-      <c r="E85" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -1860,9 +1605,6 @@
       <c r="D86" t="str">
         <v>7K</v>
       </c>
-      <c r="E86" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -1877,9 +1619,6 @@
       <c r="D87" t="str">
         <v>8B</v>
       </c>
-      <c r="E87" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -1894,9 +1633,6 @@
       <c r="D88" t="str">
         <v>8D</v>
       </c>
-      <c r="E88" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -1911,9 +1647,6 @@
       <c r="D89" t="str">
         <v>8F</v>
       </c>
-      <c r="E89" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -1928,9 +1661,6 @@
       <c r="D90" t="str">
         <v>8H</v>
       </c>
-      <c r="E90" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -1945,9 +1675,6 @@
       <c r="D91" t="str">
         <v>8J</v>
       </c>
-      <c r="E91" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -1962,9 +1689,6 @@
       <c r="D92" t="str">
         <v>9C</v>
       </c>
-      <c r="E92" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -1979,9 +1703,6 @@
       <c r="D93" t="str">
         <v>9E</v>
       </c>
-      <c r="E93" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -1996,9 +1717,6 @@
       <c r="D94" t="str">
         <v>9G</v>
       </c>
-      <c r="E94" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -2013,9 +1731,6 @@
       <c r="D95" t="str">
         <v>9I</v>
       </c>
-      <c r="E95" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -2030,9 +1745,6 @@
       <c r="D96" t="str">
         <v>9K</v>
       </c>
-      <c r="E96" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -2047,9 +1759,6 @@
       <c r="D97" t="str">
         <v>10A</v>
       </c>
-      <c r="E97" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -2064,9 +1773,6 @@
       <c r="D98" t="str">
         <v>10C</v>
       </c>
-      <c r="E98" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -2081,9 +1787,6 @@
       <c r="D99" t="str">
         <v>10E</v>
       </c>
-      <c r="E99" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -2098,9 +1801,6 @@
       <c r="D100" t="str">
         <v>10G</v>
       </c>
-      <c r="E100" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -2115,9 +1815,6 @@
       <c r="D101" t="str">
         <v>10I</v>
       </c>
-      <c r="E101" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102">
@@ -2132,9 +1829,6 @@
       <c r="D102" t="str">
         <v>10K</v>
       </c>
-      <c r="E102" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103">
@@ -2149,9 +1843,6 @@
       <c r="D103" t="str">
         <v>1A</v>
       </c>
-      <c r="E103" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104">
@@ -2166,9 +1857,6 @@
       <c r="D104" t="str">
         <v>1C</v>
       </c>
-      <c r="E104" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105">
@@ -2183,9 +1871,6 @@
       <c r="D105" t="str">
         <v>1E</v>
       </c>
-      <c r="E105" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -2200,9 +1885,6 @@
       <c r="D106" t="str">
         <v>1G</v>
       </c>
-      <c r="E106" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -2217,9 +1899,6 @@
       <c r="D107" t="str">
         <v>1I</v>
       </c>
-      <c r="E107" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108">
@@ -2234,9 +1913,6 @@
       <c r="D108" t="str">
         <v>1K</v>
       </c>
-      <c r="E108" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109">
@@ -2251,9 +1927,6 @@
       <c r="D109" t="str">
         <v>2B</v>
       </c>
-      <c r="E109" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110">
@@ -2268,9 +1941,6 @@
       <c r="D110" t="str">
         <v>2D</v>
       </c>
-      <c r="E110" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111">
@@ -2285,9 +1955,6 @@
       <c r="D111" t="str">
         <v>2F</v>
       </c>
-      <c r="E111" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112">
@@ -2302,9 +1969,6 @@
       <c r="D112" t="str">
         <v>2H</v>
       </c>
-      <c r="E112" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -2319,9 +1983,6 @@
       <c r="D113" t="str">
         <v>2J</v>
       </c>
-      <c r="E113" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114">
@@ -2336,9 +1997,6 @@
       <c r="D114" t="str">
         <v>2L</v>
       </c>
-      <c r="E114" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115">
@@ -2353,9 +2011,6 @@
       <c r="D115" t="str">
         <v>3C</v>
       </c>
-      <c r="E115" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116">
@@ -2370,9 +2025,6 @@
       <c r="D116" t="str">
         <v>3E</v>
       </c>
-      <c r="E116" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117">
@@ -2387,9 +2039,6 @@
       <c r="D117" t="str">
         <v>3G</v>
       </c>
-      <c r="E117" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118">
@@ -2404,9 +2053,6 @@
       <c r="D118" t="str">
         <v>3I</v>
       </c>
-      <c r="E118" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119">
@@ -2421,9 +2067,6 @@
       <c r="D119" t="str">
         <v>3K</v>
       </c>
-      <c r="E119" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120">
@@ -2438,9 +2081,6 @@
       <c r="D120" t="str">
         <v>4A</v>
       </c>
-      <c r="E120" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121">
@@ -2455,9 +2095,6 @@
       <c r="D121" t="str">
         <v>4C</v>
       </c>
-      <c r="E121" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122">
@@ -2472,9 +2109,6 @@
       <c r="D122" t="str">
         <v>4E</v>
       </c>
-      <c r="E122" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123">
@@ -2489,9 +2123,6 @@
       <c r="D123" t="str">
         <v>4G</v>
       </c>
-      <c r="E123" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124">
@@ -2506,9 +2137,6 @@
       <c r="D124" t="str">
         <v>4I</v>
       </c>
-      <c r="E124" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125">
@@ -2523,9 +2151,6 @@
       <c r="D125" t="str">
         <v>4K</v>
       </c>
-      <c r="E125" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126">
@@ -2540,9 +2165,6 @@
       <c r="D126" t="str">
         <v>5B</v>
       </c>
-      <c r="E126" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127">
@@ -2557,9 +2179,6 @@
       <c r="D127" t="str">
         <v>5D</v>
       </c>
-      <c r="E127" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128">
@@ -2574,9 +2193,6 @@
       <c r="D128" t="str">
         <v>5F</v>
       </c>
-      <c r="E128" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129">
@@ -2591,9 +2207,6 @@
       <c r="D129" t="str">
         <v>5H</v>
       </c>
-      <c r="E129" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130">
@@ -2608,9 +2221,6 @@
       <c r="D130" t="str">
         <v>5J</v>
       </c>
-      <c r="E130" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131">
@@ -2625,9 +2235,6 @@
       <c r="D131" t="str">
         <v>5L</v>
       </c>
-      <c r="E131" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132">
@@ -2642,9 +2249,6 @@
       <c r="D132" t="str">
         <v>6C</v>
       </c>
-      <c r="E132" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133">
@@ -2659,9 +2263,6 @@
       <c r="D133" t="str">
         <v>6E</v>
       </c>
-      <c r="E133" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134">
@@ -2676,9 +2277,6 @@
       <c r="D134" t="str">
         <v>6G</v>
       </c>
-      <c r="E134" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135">
@@ -2693,9 +2291,6 @@
       <c r="D135" t="str">
         <v>6I</v>
       </c>
-      <c r="E135" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136">
@@ -2710,9 +2305,6 @@
       <c r="D136" t="str">
         <v>6K</v>
       </c>
-      <c r="E136" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137">
@@ -2727,9 +2319,6 @@
       <c r="D137" t="str">
         <v>7A</v>
       </c>
-      <c r="E137" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138">
@@ -2744,9 +2333,6 @@
       <c r="D138" t="str">
         <v>7C</v>
       </c>
-      <c r="E138" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139">
@@ -2761,9 +2347,6 @@
       <c r="D139" t="str">
         <v>7E</v>
       </c>
-      <c r="E139" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140">
@@ -2778,9 +2361,6 @@
       <c r="D140" t="str">
         <v>7G</v>
       </c>
-      <c r="E140" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141">
@@ -2795,9 +2375,6 @@
       <c r="D141" t="str">
         <v>7I</v>
       </c>
-      <c r="E141" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142">
@@ -2812,9 +2389,6 @@
       <c r="D142" t="str">
         <v>7K</v>
       </c>
-      <c r="E142" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143">
@@ -2829,9 +2403,6 @@
       <c r="D143" t="str">
         <v>8B</v>
       </c>
-      <c r="E143" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144">
@@ -2846,9 +2417,6 @@
       <c r="D144" t="str">
         <v>8D</v>
       </c>
-      <c r="E144" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145">
@@ -2863,9 +2431,6 @@
       <c r="D145" t="str">
         <v>8F</v>
       </c>
-      <c r="E145" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146">
@@ -2880,9 +2445,6 @@
       <c r="D146" t="str">
         <v>8H</v>
       </c>
-      <c r="E146" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147">
@@ -2897,9 +2459,6 @@
       <c r="D147" t="str">
         <v>8J</v>
       </c>
-      <c r="E147" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148">
@@ -2914,9 +2473,6 @@
       <c r="D148" t="str">
         <v>8L</v>
       </c>
-      <c r="E148" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149">
@@ -2931,9 +2487,6 @@
       <c r="D149" t="str">
         <v>9C</v>
       </c>
-      <c r="E149" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150">
@@ -2948,9 +2501,6 @@
       <c r="D150" t="str">
         <v>9E</v>
       </c>
-      <c r="E150" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151">
@@ -2965,9 +2515,6 @@
       <c r="D151" t="str">
         <v>9G</v>
       </c>
-      <c r="E151" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152">
@@ -2982,9 +2529,6 @@
       <c r="D152" t="str">
         <v>9I</v>
       </c>
-      <c r="E152" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153">
@@ -2999,9 +2543,6 @@
       <c r="D153" t="str">
         <v>9K</v>
       </c>
-      <c r="E153" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154">
@@ -3016,9 +2557,6 @@
       <c r="D154" t="str">
         <v>10A</v>
       </c>
-      <c r="E154" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155">
@@ -3033,9 +2571,6 @@
       <c r="D155" t="str">
         <v>10C</v>
       </c>
-      <c r="E155" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156">
@@ -3050,9 +2585,6 @@
       <c r="D156" t="str">
         <v>10E</v>
       </c>
-      <c r="E156" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157">
@@ -3067,9 +2599,6 @@
       <c r="D157" t="str">
         <v>10G</v>
       </c>
-      <c r="E157" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="158">
       <c r="A158">
@@ -3084,9 +2613,6 @@
       <c r="D158" t="str">
         <v>10I</v>
       </c>
-      <c r="E158" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159">
@@ -3101,9 +2627,6 @@
       <c r="D159" t="str">
         <v>10K</v>
       </c>
-      <c r="E159" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160">
@@ -3118,9 +2641,6 @@
       <c r="D160" t="str">
         <v>1A</v>
       </c>
-      <c r="E160" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161">
@@ -3135,9 +2655,6 @@
       <c r="D161" t="str">
         <v>1C</v>
       </c>
-      <c r="E161" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162">
@@ -3152,9 +2669,6 @@
       <c r="D162" t="str">
         <v>1E</v>
       </c>
-      <c r="E162" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163">
@@ -3169,9 +2683,6 @@
       <c r="D163" t="str">
         <v>1G</v>
       </c>
-      <c r="E163" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164">
@@ -3186,9 +2697,6 @@
       <c r="D164" t="str">
         <v>1I</v>
       </c>
-      <c r="E164" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165">
@@ -3203,9 +2711,6 @@
       <c r="D165" t="str">
         <v>1K</v>
       </c>
-      <c r="E165" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166">
@@ -3220,9 +2725,6 @@
       <c r="D166" t="str">
         <v>1M</v>
       </c>
-      <c r="E166" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167">
@@ -3237,9 +2739,6 @@
       <c r="D167" t="str">
         <v>2B</v>
       </c>
-      <c r="E167" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168">
@@ -3254,9 +2753,6 @@
       <c r="D168" t="str">
         <v>2D</v>
       </c>
-      <c r="E168" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="169">
       <c r="A169">
@@ -3271,9 +2767,6 @@
       <c r="D169" t="str">
         <v>2F</v>
       </c>
-      <c r="E169" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170">
@@ -3288,9 +2781,6 @@
       <c r="D170" t="str">
         <v>2H</v>
       </c>
-      <c r="E170" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171">
@@ -3305,9 +2795,6 @@
       <c r="D171" t="str">
         <v>2J</v>
       </c>
-      <c r="E171" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172">
@@ -3322,9 +2809,6 @@
       <c r="D172" t="str">
         <v>2L</v>
       </c>
-      <c r="E172" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173">
@@ -3339,9 +2823,6 @@
       <c r="D173" t="str">
         <v>3C</v>
       </c>
-      <c r="E173" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174">
@@ -3356,9 +2837,6 @@
       <c r="D174" t="str">
         <v>3E</v>
       </c>
-      <c r="E174" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="175">
       <c r="A175">
@@ -3373,9 +2851,6 @@
       <c r="D175" t="str">
         <v>3G</v>
       </c>
-      <c r="E175" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176">
@@ -3390,9 +2865,6 @@
       <c r="D176" t="str">
         <v>3I</v>
       </c>
-      <c r="E176" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177">
@@ -3407,9 +2879,6 @@
       <c r="D177" t="str">
         <v>3K</v>
       </c>
-      <c r="E177" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178">
@@ -3424,9 +2893,6 @@
       <c r="D178" t="str">
         <v>3M</v>
       </c>
-      <c r="E178" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179">
@@ -3441,9 +2907,6 @@
       <c r="D179" t="str">
         <v>4A</v>
       </c>
-      <c r="E179" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180">
@@ -3458,9 +2921,6 @@
       <c r="D180" t="str">
         <v>4C</v>
       </c>
-      <c r="E180" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181">
@@ -3475,9 +2935,6 @@
       <c r="D181" t="str">
         <v>4E</v>
       </c>
-      <c r="E181" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182">
@@ -3492,9 +2949,6 @@
       <c r="D182" t="str">
         <v>4G</v>
       </c>
-      <c r="E182" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183">
@@ -3509,9 +2963,6 @@
       <c r="D183" t="str">
         <v>4I</v>
       </c>
-      <c r="E183" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184">
@@ -3526,9 +2977,6 @@
       <c r="D184" t="str">
         <v>4K</v>
       </c>
-      <c r="E184" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185">
@@ -3543,9 +2991,6 @@
       <c r="D185" t="str">
         <v>4M</v>
       </c>
-      <c r="E185" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186">
@@ -3560,9 +3005,6 @@
       <c r="D186" t="str">
         <v>5B</v>
       </c>
-      <c r="E186" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187">
@@ -3577,9 +3019,6 @@
       <c r="D187" t="str">
         <v>5D</v>
       </c>
-      <c r="E187" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188">
@@ -3594,9 +3033,6 @@
       <c r="D188" t="str">
         <v>5F</v>
       </c>
-      <c r="E188" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189">
@@ -3611,9 +3047,6 @@
       <c r="D189" t="str">
         <v>5H</v>
       </c>
-      <c r="E189" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="190">
       <c r="A190">
@@ -3628,9 +3061,6 @@
       <c r="D190" t="str">
         <v>5J</v>
       </c>
-      <c r="E190" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191">
@@ -3645,9 +3075,6 @@
       <c r="D191" t="str">
         <v>5L</v>
       </c>
-      <c r="E191" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192">
@@ -3662,9 +3089,6 @@
       <c r="D192" t="str">
         <v>6C</v>
       </c>
-      <c r="E192" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193">
@@ -3679,9 +3103,6 @@
       <c r="D193" t="str">
         <v>6E</v>
       </c>
-      <c r="E193" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194">
@@ -3696,9 +3117,6 @@
       <c r="D194" t="str">
         <v>6G</v>
       </c>
-      <c r="E194" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195">
@@ -3713,9 +3131,6 @@
       <c r="D195" t="str">
         <v>6I</v>
       </c>
-      <c r="E195" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196">
@@ -3730,9 +3145,6 @@
       <c r="D196" t="str">
         <v>6K</v>
       </c>
-      <c r="E196" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197">
@@ -3747,9 +3159,6 @@
       <c r="D197" t="str">
         <v>6M</v>
       </c>
-      <c r="E197" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198">
@@ -3764,9 +3173,6 @@
       <c r="D198" t="str">
         <v>7A</v>
       </c>
-      <c r="E198" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199">
@@ -3781,9 +3187,6 @@
       <c r="D199" t="str">
         <v>7C</v>
       </c>
-      <c r="E199" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200">
@@ -3798,9 +3201,6 @@
       <c r="D200" t="str">
         <v>7E</v>
       </c>
-      <c r="E200" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201">
@@ -3815,9 +3215,6 @@
       <c r="D201" t="str">
         <v>7G</v>
       </c>
-      <c r="E201" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202">
@@ -3832,9 +3229,6 @@
       <c r="D202" t="str">
         <v>7I</v>
       </c>
-      <c r="E202" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203">
@@ -3849,9 +3243,6 @@
       <c r="D203" t="str">
         <v>7K</v>
       </c>
-      <c r="E203" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204">
@@ -3866,9 +3257,6 @@
       <c r="D204" t="str">
         <v>7M</v>
       </c>
-      <c r="E204" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205">
@@ -3883,9 +3271,6 @@
       <c r="D205" t="str">
         <v>8B</v>
       </c>
-      <c r="E205" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206">
@@ -3900,9 +3285,6 @@
       <c r="D206" t="str">
         <v>8D</v>
       </c>
-      <c r="E206" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207">
@@ -3917,9 +3299,6 @@
       <c r="D207" t="str">
         <v>8F</v>
       </c>
-      <c r="E207" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208">
@@ -3934,9 +3313,6 @@
       <c r="D208" t="str">
         <v>8H</v>
       </c>
-      <c r="E208" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209">
@@ -3951,9 +3327,6 @@
       <c r="D209" t="str">
         <v>8J</v>
       </c>
-      <c r="E209" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210">
@@ -3968,9 +3341,6 @@
       <c r="D210" t="str">
         <v>8L</v>
       </c>
-      <c r="E210" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211">
@@ -3985,9 +3355,6 @@
       <c r="D211" t="str">
         <v>9C</v>
       </c>
-      <c r="E211" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212">
@@ -4002,9 +3369,6 @@
       <c r="D212" t="str">
         <v>9E</v>
       </c>
-      <c r="E212" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213">
@@ -4019,9 +3383,6 @@
       <c r="D213" t="str">
         <v>9G</v>
       </c>
-      <c r="E213" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214">
@@ -4036,9 +3397,6 @@
       <c r="D214" t="str">
         <v>9I</v>
       </c>
-      <c r="E214" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215">
@@ -4053,9 +3411,6 @@
       <c r="D215" t="str">
         <v>9K</v>
       </c>
-      <c r="E215" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216">
@@ -4070,9 +3425,6 @@
       <c r="D216" t="str">
         <v>9M</v>
       </c>
-      <c r="E216" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217">
@@ -4087,9 +3439,6 @@
       <c r="D217" t="str">
         <v>10A</v>
       </c>
-      <c r="E217" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218">
@@ -4104,9 +3453,6 @@
       <c r="D218" t="str">
         <v>10C</v>
       </c>
-      <c r="E218" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219">
@@ -4121,9 +3467,6 @@
       <c r="D219" t="str">
         <v>10E</v>
       </c>
-      <c r="E219" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220">
@@ -4138,9 +3481,6 @@
       <c r="D220" t="str">
         <v>10G</v>
       </c>
-      <c r="E220" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221">
@@ -4155,9 +3495,6 @@
       <c r="D221" t="str">
         <v>10I</v>
       </c>
-      <c r="E221" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222">
@@ -4172,9 +3509,6 @@
       <c r="D222" t="str">
         <v>10K</v>
       </c>
-      <c r="E222" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223">
@@ -4189,9 +3523,6 @@
       <c r="D223" t="str">
         <v>10M</v>
       </c>
-      <c r="E223" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224">
@@ -4206,9 +3537,6 @@
       <c r="D224" t="str">
         <v>1A</v>
       </c>
-      <c r="E224" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225">
@@ -4223,9 +3551,6 @@
       <c r="D225" t="str">
         <v>1C</v>
       </c>
-      <c r="E225" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226">
@@ -4240,9 +3565,6 @@
       <c r="D226" t="str">
         <v>1E</v>
       </c>
-      <c r="E226" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227">
@@ -4257,9 +3579,6 @@
       <c r="D227" t="str">
         <v>1G</v>
       </c>
-      <c r="E227" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228">
@@ -4274,9 +3593,6 @@
       <c r="D228" t="str">
         <v>1I</v>
       </c>
-      <c r="E228" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229">
@@ -4291,9 +3607,6 @@
       <c r="D229" t="str">
         <v>1K</v>
       </c>
-      <c r="E229" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230">
@@ -4308,9 +3621,6 @@
       <c r="D230" t="str">
         <v>1M</v>
       </c>
-      <c r="E230" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231">
@@ -4325,9 +3635,6 @@
       <c r="D231" t="str">
         <v>2B</v>
       </c>
-      <c r="E231" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="232">
       <c r="A232">
@@ -4342,9 +3649,6 @@
       <c r="D232" t="str">
         <v>2D</v>
       </c>
-      <c r="E232" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233">
@@ -4359,9 +3663,6 @@
       <c r="D233" t="str">
         <v>2F</v>
       </c>
-      <c r="E233" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="234">
       <c r="A234">
@@ -4376,9 +3677,6 @@
       <c r="D234" t="str">
         <v>2H</v>
       </c>
-      <c r="E234" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235">
@@ -4393,9 +3691,6 @@
       <c r="D235" t="str">
         <v>2J</v>
       </c>
-      <c r="E235" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236">
@@ -4410,9 +3705,6 @@
       <c r="D236" t="str">
         <v>2L</v>
       </c>
-      <c r="E236" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237">
@@ -4427,9 +3719,6 @@
       <c r="D237" t="str">
         <v>2N</v>
       </c>
-      <c r="E237" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238">
@@ -4444,9 +3733,6 @@
       <c r="D238" t="str">
         <v>3C</v>
       </c>
-      <c r="E238" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239">
@@ -4461,9 +3747,6 @@
       <c r="D239" t="str">
         <v>3E</v>
       </c>
-      <c r="E239" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240">
@@ -4478,9 +3761,6 @@
       <c r="D240" t="str">
         <v>3G</v>
       </c>
-      <c r="E240" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241">
@@ -4495,9 +3775,6 @@
       <c r="D241" t="str">
         <v>3I</v>
       </c>
-      <c r="E241" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242">
@@ -4512,9 +3789,6 @@
       <c r="D242" t="str">
         <v>3K</v>
       </c>
-      <c r="E242" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243">
@@ -4529,9 +3803,6 @@
       <c r="D243" t="str">
         <v>3M</v>
       </c>
-      <c r="E243" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244">
@@ -4546,9 +3817,6 @@
       <c r="D244" t="str">
         <v>4A</v>
       </c>
-      <c r="E244" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245">
@@ -4563,9 +3831,6 @@
       <c r="D245" t="str">
         <v>4C</v>
       </c>
-      <c r="E245" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="246">
       <c r="A246">
@@ -4580,9 +3845,6 @@
       <c r="D246" t="str">
         <v>4E</v>
       </c>
-      <c r="E246" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247">
@@ -4597,9 +3859,6 @@
       <c r="D247" t="str">
         <v>4G</v>
       </c>
-      <c r="E247" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248">
@@ -4614,9 +3873,6 @@
       <c r="D248" t="str">
         <v>4I</v>
       </c>
-      <c r="E248" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="249">
       <c r="A249">
@@ -4631,9 +3887,6 @@
       <c r="D249" t="str">
         <v>4K</v>
       </c>
-      <c r="E249" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="250">
       <c r="A250">
@@ -4648,9 +3901,6 @@
       <c r="D250" t="str">
         <v>4M</v>
       </c>
-      <c r="E250" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="251">
       <c r="A251">
@@ -4665,9 +3915,6 @@
       <c r="D251" t="str">
         <v>5B</v>
       </c>
-      <c r="E251" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="252">
       <c r="A252">
@@ -4682,9 +3929,6 @@
       <c r="D252" t="str">
         <v>5D</v>
       </c>
-      <c r="E252" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="253">
       <c r="A253">
@@ -4699,9 +3943,6 @@
       <c r="D253" t="str">
         <v>5F</v>
       </c>
-      <c r="E253" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="254">
       <c r="A254">
@@ -4716,9 +3957,6 @@
       <c r="D254" t="str">
         <v>5H</v>
       </c>
-      <c r="E254" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="255">
       <c r="A255">
@@ -4733,9 +3971,6 @@
       <c r="D255" t="str">
         <v>5J</v>
       </c>
-      <c r="E255" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="256">
       <c r="A256">
@@ -4750,9 +3985,6 @@
       <c r="D256" t="str">
         <v>5L</v>
       </c>
-      <c r="E256" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="257">
       <c r="A257">
@@ -4767,9 +3999,6 @@
       <c r="D257" t="str">
         <v>5N</v>
       </c>
-      <c r="E257" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="258">
       <c r="A258">
@@ -4784,9 +4013,6 @@
       <c r="D258" t="str">
         <v>6C</v>
       </c>
-      <c r="E258" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="259">
       <c r="A259">
@@ -4801,9 +4027,6 @@
       <c r="D259" t="str">
         <v>6E</v>
       </c>
-      <c r="E259" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="260">
       <c r="A260">
@@ -4818,9 +4041,6 @@
       <c r="D260" t="str">
         <v>6G</v>
       </c>
-      <c r="E260" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="261">
       <c r="A261">
@@ -4835,9 +4055,6 @@
       <c r="D261" t="str">
         <v>6I</v>
       </c>
-      <c r="E261" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="262">
       <c r="A262">
@@ -4852,9 +4069,6 @@
       <c r="D262" t="str">
         <v>6K</v>
       </c>
-      <c r="E262" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="263">
       <c r="A263">
@@ -4869,9 +4083,6 @@
       <c r="D263" t="str">
         <v>6M</v>
       </c>
-      <c r="E263" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="264">
       <c r="A264">
@@ -4886,9 +4097,6 @@
       <c r="D264" t="str">
         <v>7A</v>
       </c>
-      <c r="E264" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="265">
       <c r="A265">
@@ -4903,9 +4111,6 @@
       <c r="D265" t="str">
         <v>7C</v>
       </c>
-      <c r="E265" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="266">
       <c r="A266">
@@ -4920,9 +4125,6 @@
       <c r="D266" t="str">
         <v>7E</v>
       </c>
-      <c r="E266" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="267">
       <c r="A267">
@@ -4937,9 +4139,6 @@
       <c r="D267" t="str">
         <v>7G</v>
       </c>
-      <c r="E267" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="268">
       <c r="A268">
@@ -4954,9 +4153,6 @@
       <c r="D268" t="str">
         <v>7I</v>
       </c>
-      <c r="E268" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="269">
       <c r="A269">
@@ -4971,9 +4167,6 @@
       <c r="D269" t="str">
         <v>7K</v>
       </c>
-      <c r="E269" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="270">
       <c r="A270">
@@ -4988,9 +4181,6 @@
       <c r="D270" t="str">
         <v>7M</v>
       </c>
-      <c r="E270" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="271">
       <c r="A271">
@@ -5005,9 +4195,6 @@
       <c r="D271" t="str">
         <v>8B</v>
       </c>
-      <c r="E271" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="272">
       <c r="A272">
@@ -5022,9 +4209,6 @@
       <c r="D272" t="str">
         <v>8D</v>
       </c>
-      <c r="E272" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="273">
       <c r="A273">
@@ -5039,9 +4223,6 @@
       <c r="D273" t="str">
         <v>8F</v>
       </c>
-      <c r="E273" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="274">
       <c r="A274">
@@ -5056,9 +4237,6 @@
       <c r="D274" t="str">
         <v>8H</v>
       </c>
-      <c r="E274" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="275">
       <c r="A275">
@@ -5073,9 +4251,6 @@
       <c r="D275" t="str">
         <v>8J</v>
       </c>
-      <c r="E275" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="276">
       <c r="A276">
@@ -5090,9 +4265,6 @@
       <c r="D276" t="str">
         <v>8L</v>
       </c>
-      <c r="E276" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="277">
       <c r="A277">
@@ -5107,9 +4279,6 @@
       <c r="D277" t="str">
         <v>8N</v>
       </c>
-      <c r="E277" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="278">
       <c r="A278">
@@ -5124,9 +4293,6 @@
       <c r="D278" t="str">
         <v>9C</v>
       </c>
-      <c r="E278" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="279">
       <c r="A279">
@@ -5141,9 +4307,6 @@
       <c r="D279" t="str">
         <v>9E</v>
       </c>
-      <c r="E279" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="280">
       <c r="A280">
@@ -5158,9 +4321,6 @@
       <c r="D280" t="str">
         <v>9G</v>
       </c>
-      <c r="E280" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="281">
       <c r="A281">
@@ -5175,9 +4335,6 @@
       <c r="D281" t="str">
         <v>9I</v>
       </c>
-      <c r="E281" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="282">
       <c r="A282">
@@ -5192,9 +4349,6 @@
       <c r="D282" t="str">
         <v>9K</v>
       </c>
-      <c r="E282" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="283">
       <c r="A283">
@@ -5209,9 +4363,6 @@
       <c r="D283" t="str">
         <v>9M</v>
       </c>
-      <c r="E283" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="284">
       <c r="A284">
@@ -5226,9 +4377,6 @@
       <c r="D284" t="str">
         <v>10A</v>
       </c>
-      <c r="E284" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="285">
       <c r="A285">
@@ -5243,9 +4391,6 @@
       <c r="D285" t="str">
         <v>10C</v>
       </c>
-      <c r="E285" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="286">
       <c r="A286">
@@ -5260,9 +4405,6 @@
       <c r="D286" t="str">
         <v>10E</v>
       </c>
-      <c r="E286" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="287">
       <c r="A287">
@@ -5277,9 +4419,6 @@
       <c r="D287" t="str">
         <v>10G</v>
       </c>
-      <c r="E287" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="288">
       <c r="A288">
@@ -5294,9 +4433,6 @@
       <c r="D288" t="str">
         <v>10I</v>
       </c>
-      <c r="E288" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="289">
       <c r="A289">
@@ -5311,9 +4447,6 @@
       <c r="D289" t="str">
         <v>10K</v>
       </c>
-      <c r="E289" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="290">
       <c r="A290">
@@ -5328,9 +4461,6 @@
       <c r="D290" t="str">
         <v>10M</v>
       </c>
-      <c r="E290" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="291">
       <c r="A291">
@@ -5345,9 +4475,6 @@
       <c r="D291" t="str">
         <v>1A</v>
       </c>
-      <c r="E291" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="292">
       <c r="A292">
@@ -5362,9 +4489,6 @@
       <c r="D292" t="str">
         <v>1C</v>
       </c>
-      <c r="E292" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="293">
       <c r="A293">
@@ -5379,9 +4503,6 @@
       <c r="D293" t="str">
         <v>1E</v>
       </c>
-      <c r="E293" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="294">
       <c r="A294">
@@ -5396,9 +4517,6 @@
       <c r="D294" t="str">
         <v>1G</v>
       </c>
-      <c r="E294" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="295">
       <c r="A295">
@@ -5413,9 +4531,6 @@
       <c r="D295" t="str">
         <v>1I</v>
       </c>
-      <c r="E295" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="296">
       <c r="A296">
@@ -5430,9 +4545,6 @@
       <c r="D296" t="str">
         <v>1K</v>
       </c>
-      <c r="E296" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="297">
       <c r="A297">
@@ -5447,9 +4559,6 @@
       <c r="D297" t="str">
         <v>1M</v>
       </c>
-      <c r="E297" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="298">
       <c r="A298">
@@ -5464,9 +4573,6 @@
       <c r="D298" t="str">
         <v>1O</v>
       </c>
-      <c r="E298" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="299">
       <c r="A299">
@@ -5481,9 +4587,6 @@
       <c r="D299" t="str">
         <v>2B</v>
       </c>
-      <c r="E299" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="300">
       <c r="A300">
@@ -5498,9 +4601,6 @@
       <c r="D300" t="str">
         <v>2D</v>
       </c>
-      <c r="E300" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="301">
       <c r="A301">
@@ -5515,9 +4615,6 @@
       <c r="D301" t="str">
         <v>2F</v>
       </c>
-      <c r="E301" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="302">
       <c r="A302">
@@ -5532,9 +4629,6 @@
       <c r="D302" t="str">
         <v>2H</v>
       </c>
-      <c r="E302" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="303">
       <c r="A303">
@@ -5549,9 +4643,6 @@
       <c r="D303" t="str">
         <v>2J</v>
       </c>
-      <c r="E303" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="304">
       <c r="A304">
@@ -5566,9 +4657,6 @@
       <c r="D304" t="str">
         <v>2L</v>
       </c>
-      <c r="E304" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="305">
       <c r="A305">
@@ -5583,9 +4671,6 @@
       <c r="D305" t="str">
         <v>2N</v>
       </c>
-      <c r="E305" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="306">
       <c r="A306">
@@ -5600,9 +4685,6 @@
       <c r="D306" t="str">
         <v>3C</v>
       </c>
-      <c r="E306" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="307">
       <c r="A307">
@@ -5617,9 +4699,6 @@
       <c r="D307" t="str">
         <v>3E</v>
       </c>
-      <c r="E307" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="308">
       <c r="A308">
@@ -5634,9 +4713,6 @@
       <c r="D308" t="str">
         <v>3G</v>
       </c>
-      <c r="E308" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="309">
       <c r="A309">
@@ -5651,9 +4727,6 @@
       <c r="D309" t="str">
         <v>3I</v>
       </c>
-      <c r="E309" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="310">
       <c r="A310">
@@ -5668,9 +4741,6 @@
       <c r="D310" t="str">
         <v>3K</v>
       </c>
-      <c r="E310" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="311">
       <c r="A311">
@@ -5685,9 +4755,6 @@
       <c r="D311" t="str">
         <v>3M</v>
       </c>
-      <c r="E311" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="312">
       <c r="A312">
@@ -5702,9 +4769,6 @@
       <c r="D312" t="str">
         <v>3O</v>
       </c>
-      <c r="E312" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="313">
       <c r="A313">
@@ -5719,9 +4783,6 @@
       <c r="D313" t="str">
         <v>4A</v>
       </c>
-      <c r="E313" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="314">
       <c r="A314">
@@ -5736,9 +4797,6 @@
       <c r="D314" t="str">
         <v>4C</v>
       </c>
-      <c r="E314" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="315">
       <c r="A315">
@@ -5753,9 +4811,6 @@
       <c r="D315" t="str">
         <v>4E</v>
       </c>
-      <c r="E315" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="316">
       <c r="A316">
@@ -5770,9 +4825,6 @@
       <c r="D316" t="str">
         <v>4G</v>
       </c>
-      <c r="E316" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="317">
       <c r="A317">
@@ -5787,9 +4839,6 @@
       <c r="D317" t="str">
         <v>4I</v>
       </c>
-      <c r="E317" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="318">
       <c r="A318">
@@ -5804,9 +4853,6 @@
       <c r="D318" t="str">
         <v>4K</v>
       </c>
-      <c r="E318" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="319">
       <c r="A319">
@@ -5821,9 +4867,6 @@
       <c r="D319" t="str">
         <v>4M</v>
       </c>
-      <c r="E319" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="320">
       <c r="A320">
@@ -5838,9 +4881,6 @@
       <c r="D320" t="str">
         <v>4O</v>
       </c>
-      <c r="E320" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="321">
       <c r="A321">
@@ -5855,9 +4895,6 @@
       <c r="D321" t="str">
         <v>5B</v>
       </c>
-      <c r="E321" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="322">
       <c r="A322">
@@ -5872,9 +4909,6 @@
       <c r="D322" t="str">
         <v>5D</v>
       </c>
-      <c r="E322" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="323">
       <c r="A323">
@@ -5889,9 +4923,6 @@
       <c r="D323" t="str">
         <v>5F</v>
       </c>
-      <c r="E323" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="324">
       <c r="A324">
@@ -5906,9 +4937,6 @@
       <c r="D324" t="str">
         <v>5H</v>
       </c>
-      <c r="E324" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="325">
       <c r="A325">
@@ -5923,9 +4951,6 @@
       <c r="D325" t="str">
         <v>5J</v>
       </c>
-      <c r="E325" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="326">
       <c r="A326">
@@ -5940,9 +4965,6 @@
       <c r="D326" t="str">
         <v>5L</v>
       </c>
-      <c r="E326" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="327">
       <c r="A327">
@@ -5957,9 +4979,6 @@
       <c r="D327" t="str">
         <v>5N</v>
       </c>
-      <c r="E327" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="328">
       <c r="A328">
@@ -5974,9 +4993,6 @@
       <c r="D328" t="str">
         <v>6C</v>
       </c>
-      <c r="E328" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="329">
       <c r="A329">
@@ -5991,9 +5007,6 @@
       <c r="D329" t="str">
         <v>6E</v>
       </c>
-      <c r="E329" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="330">
       <c r="A330">
@@ -6008,9 +5021,6 @@
       <c r="D330" t="str">
         <v>6G</v>
       </c>
-      <c r="E330" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="331">
       <c r="A331">
@@ -6025,9 +5035,6 @@
       <c r="D331" t="str">
         <v>6I</v>
       </c>
-      <c r="E331" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="332">
       <c r="A332">
@@ -6042,9 +5049,6 @@
       <c r="D332" t="str">
         <v>6K</v>
       </c>
-      <c r="E332" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="333">
       <c r="A333">
@@ -6059,9 +5063,6 @@
       <c r="D333" t="str">
         <v>6M</v>
       </c>
-      <c r="E333" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="334">
       <c r="A334">
@@ -6076,9 +5077,6 @@
       <c r="D334" t="str">
         <v>6O</v>
       </c>
-      <c r="E334" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="335">
       <c r="A335">
@@ -6093,9 +5091,6 @@
       <c r="D335" t="str">
         <v>7A</v>
       </c>
-      <c r="E335" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="336">
       <c r="A336">
@@ -6110,9 +5105,6 @@
       <c r="D336" t="str">
         <v>7C</v>
       </c>
-      <c r="E336" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="337">
       <c r="A337">
@@ -6127,9 +5119,6 @@
       <c r="D337" t="str">
         <v>7E</v>
       </c>
-      <c r="E337" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="338">
       <c r="A338">
@@ -6144,9 +5133,6 @@
       <c r="D338" t="str">
         <v>7G</v>
       </c>
-      <c r="E338" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="339">
       <c r="A339">
@@ -6161,9 +5147,6 @@
       <c r="D339" t="str">
         <v>7I</v>
       </c>
-      <c r="E339" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="340">
       <c r="A340">
@@ -6178,9 +5161,6 @@
       <c r="D340" t="str">
         <v>7K</v>
       </c>
-      <c r="E340" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="341">
       <c r="A341">
@@ -6195,9 +5175,6 @@
       <c r="D341" t="str">
         <v>7M</v>
       </c>
-      <c r="E341" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="342">
       <c r="A342">
@@ -6212,9 +5189,6 @@
       <c r="D342" t="str">
         <v>7O</v>
       </c>
-      <c r="E342" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="343">
       <c r="A343">
@@ -6229,9 +5203,6 @@
       <c r="D343" t="str">
         <v>8B</v>
       </c>
-      <c r="E343" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="344">
       <c r="A344">
@@ -6246,9 +5217,6 @@
       <c r="D344" t="str">
         <v>8D</v>
       </c>
-      <c r="E344" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="345">
       <c r="A345">
@@ -6263,9 +5231,6 @@
       <c r="D345" t="str">
         <v>8F</v>
       </c>
-      <c r="E345" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="346">
       <c r="A346">
@@ -6280,9 +5245,6 @@
       <c r="D346" t="str">
         <v>8H</v>
       </c>
-      <c r="E346" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="347">
       <c r="A347">
@@ -6297,9 +5259,6 @@
       <c r="D347" t="str">
         <v>8J</v>
       </c>
-      <c r="E347" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="348">
       <c r="A348">
@@ -6314,9 +5273,6 @@
       <c r="D348" t="str">
         <v>8L</v>
       </c>
-      <c r="E348" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="349">
       <c r="A349">
@@ -6331,9 +5287,6 @@
       <c r="D349" t="str">
         <v>8N</v>
       </c>
-      <c r="E349" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="350">
       <c r="A350">
@@ -6348,9 +5301,6 @@
       <c r="D350" t="str">
         <v>9C</v>
       </c>
-      <c r="E350" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="351">
       <c r="A351">
@@ -6365,9 +5315,6 @@
       <c r="D351" t="str">
         <v>9E</v>
       </c>
-      <c r="E351" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="352">
       <c r="A352">
@@ -6382,9 +5329,6 @@
       <c r="D352" t="str">
         <v>9G</v>
       </c>
-      <c r="E352" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="353">
       <c r="A353">
@@ -6399,9 +5343,6 @@
       <c r="D353" t="str">
         <v>9I</v>
       </c>
-      <c r="E353" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="354">
       <c r="A354">
@@ -6416,9 +5357,6 @@
       <c r="D354" t="str">
         <v>9K</v>
       </c>
-      <c r="E354" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="355">
       <c r="A355">
@@ -6433,9 +5371,6 @@
       <c r="D355" t="str">
         <v>9M</v>
       </c>
-      <c r="E355" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="356">
       <c r="A356">
@@ -6450,9 +5385,6 @@
       <c r="D356" t="str">
         <v>9O</v>
       </c>
-      <c r="E356" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="357">
       <c r="A357">
@@ -6467,9 +5399,6 @@
       <c r="D357" t="str">
         <v>10A</v>
       </c>
-      <c r="E357" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="358">
       <c r="A358">
@@ -6484,9 +5413,6 @@
       <c r="D358" t="str">
         <v>10C</v>
       </c>
-      <c r="E358" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="359">
       <c r="A359">
@@ -6501,9 +5427,6 @@
       <c r="D359" t="str">
         <v>10E</v>
       </c>
-      <c r="E359" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="360">
       <c r="A360">
@@ -6518,9 +5441,6 @@
       <c r="D360" t="str">
         <v>10G</v>
       </c>
-      <c r="E360" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="361">
       <c r="A361">
@@ -6535,9 +5455,6 @@
       <c r="D361" t="str">
         <v>10I</v>
       </c>
-      <c r="E361" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="362">
       <c r="A362">
@@ -6552,9 +5469,6 @@
       <c r="D362" t="str">
         <v>10K</v>
       </c>
-      <c r="E362" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="363">
       <c r="A363">
@@ -6569,9 +5483,6 @@
       <c r="D363" t="str">
         <v>10M</v>
       </c>
-      <c r="E363" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="364">
       <c r="A364">
@@ -6586,9 +5497,6 @@
       <c r="D364" t="str">
         <v>10O</v>
       </c>
-      <c r="E364" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="365">
       <c r="A365">
@@ -6603,9 +5511,6 @@
       <c r="D365" t="str">
         <v>1A</v>
       </c>
-      <c r="E365" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="366">
       <c r="A366">
@@ -6620,9 +5525,6 @@
       <c r="D366" t="str">
         <v>1C</v>
       </c>
-      <c r="E366" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="367">
       <c r="A367">
@@ -6637,9 +5539,6 @@
       <c r="D367" t="str">
         <v>1E</v>
       </c>
-      <c r="E367" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="368">
       <c r="A368">
@@ -6654,9 +5553,6 @@
       <c r="D368" t="str">
         <v>1G</v>
       </c>
-      <c r="E368" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="369">
       <c r="A369">
@@ -6671,9 +5567,6 @@
       <c r="D369" t="str">
         <v>1I</v>
       </c>
-      <c r="E369" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="370">
       <c r="A370">
@@ -6688,9 +5581,6 @@
       <c r="D370" t="str">
         <v>1K</v>
       </c>
-      <c r="E370" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="371">
       <c r="A371">
@@ -6705,9 +5595,6 @@
       <c r="D371" t="str">
         <v>1M</v>
       </c>
-      <c r="E371" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="372">
       <c r="A372">
@@ -6722,9 +5609,6 @@
       <c r="D372" t="str">
         <v>1O</v>
       </c>
-      <c r="E372" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="373">
       <c r="A373">
@@ -6739,9 +5623,6 @@
       <c r="D373" t="str">
         <v>2B</v>
       </c>
-      <c r="E373" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="374">
       <c r="A374">
@@ -6756,9 +5637,6 @@
       <c r="D374" t="str">
         <v>2D</v>
       </c>
-      <c r="E374" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="375">
       <c r="A375">
@@ -6773,9 +5651,6 @@
       <c r="D375" t="str">
         <v>2F</v>
       </c>
-      <c r="E375" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="376">
       <c r="A376">
@@ -6790,9 +5665,6 @@
       <c r="D376" t="str">
         <v>2H</v>
       </c>
-      <c r="E376" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="377">
       <c r="A377">
@@ -6807,9 +5679,6 @@
       <c r="D377" t="str">
         <v>2J</v>
       </c>
-      <c r="E377" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="378">
       <c r="A378">
@@ -6824,9 +5693,6 @@
       <c r="D378" t="str">
         <v>2L</v>
       </c>
-      <c r="E378" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="379">
       <c r="A379">
@@ -6841,9 +5707,6 @@
       <c r="D379" t="str">
         <v>2N</v>
       </c>
-      <c r="E379" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="380">
       <c r="A380">
@@ -6858,9 +5721,6 @@
       <c r="D380" t="str">
         <v>2P</v>
       </c>
-      <c r="E380" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="381">
       <c r="A381">
@@ -6875,9 +5735,6 @@
       <c r="D381" t="str">
         <v>3C</v>
       </c>
-      <c r="E381" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="382">
       <c r="A382">
@@ -6892,9 +5749,6 @@
       <c r="D382" t="str">
         <v>3E</v>
       </c>
-      <c r="E382" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="383">
       <c r="A383">
@@ -6909,9 +5763,6 @@
       <c r="D383" t="str">
         <v>3G</v>
       </c>
-      <c r="E383" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="384">
       <c r="A384">
@@ -6926,9 +5777,6 @@
       <c r="D384" t="str">
         <v>3I</v>
       </c>
-      <c r="E384" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="385">
       <c r="A385">
@@ -6943,9 +5791,6 @@
       <c r="D385" t="str">
         <v>3K</v>
       </c>
-      <c r="E385" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="386">
       <c r="A386">
@@ -6960,9 +5805,6 @@
       <c r="D386" t="str">
         <v>3M</v>
       </c>
-      <c r="E386" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="387">
       <c r="A387">
@@ -6977,9 +5819,6 @@
       <c r="D387" t="str">
         <v>3O</v>
       </c>
-      <c r="E387" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="388">
       <c r="A388">
@@ -6994,9 +5833,6 @@
       <c r="D388" t="str">
         <v>4A</v>
       </c>
-      <c r="E388" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="389">
       <c r="A389">
@@ -7011,9 +5847,6 @@
       <c r="D389" t="str">
         <v>4C</v>
       </c>
-      <c r="E389" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="390">
       <c r="A390">
@@ -7028,9 +5861,6 @@
       <c r="D390" t="str">
         <v>4E</v>
       </c>
-      <c r="E390" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="391">
       <c r="A391">
@@ -7045,9 +5875,6 @@
       <c r="D391" t="str">
         <v>4G</v>
       </c>
-      <c r="E391" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="392">
       <c r="A392">
@@ -7062,9 +5889,6 @@
       <c r="D392" t="str">
         <v>4I</v>
       </c>
-      <c r="E392" t="str">
-        <v>horseman</v>
-      </c>
     </row>
     <row r="393">
       <c r="A393">
@@ -7079,13 +5903,10 @@
       <c r="D393" t="str">
         <v>4K</v>
       </c>
-      <c r="E393" t="str">
-        <v>horseman</v>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E393"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D393"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
getting to req raising
</commit_message>
<xml_diff>
--- a/BE/Aarrangement.xlsx
+++ b/BE/Aarrangement.xlsx
@@ -433,7 +433,7 @@
         <v>1A</v>
       </c>
       <c r="E2" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="3">
@@ -450,7 +450,7 @@
         <v>1C</v>
       </c>
       <c r="E3" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         <v>1E</v>
       </c>
       <c r="E4" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="5">
@@ -484,7 +484,7 @@
         <v>1G</v>
       </c>
       <c r="E5" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="6">
@@ -501,7 +501,7 @@
         <v>1I</v>
       </c>
       <c r="E6" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="7">
@@ -518,7 +518,7 @@
         <v>2B</v>
       </c>
       <c r="E7" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="8">
@@ -535,7 +535,7 @@
         <v>2D</v>
       </c>
       <c r="E8" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="9">
@@ -552,7 +552,7 @@
         <v>2F</v>
       </c>
       <c r="E9" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="10">
@@ -569,7 +569,7 @@
         <v>2H</v>
       </c>
       <c r="E10" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="11">
@@ -586,7 +586,7 @@
         <v>2J</v>
       </c>
       <c r="E11" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="12">
@@ -603,7 +603,7 @@
         <v>3C</v>
       </c>
       <c r="E12" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="13">
@@ -620,7 +620,7 @@
         <v>3E</v>
       </c>
       <c r="E13" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="14">
@@ -637,7 +637,7 @@
         <v>3G</v>
       </c>
       <c r="E14" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="15">
@@ -654,7 +654,7 @@
         <v>3I</v>
       </c>
       <c r="E15" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="16">
@@ -671,7 +671,7 @@
         <v>4A</v>
       </c>
       <c r="E16" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="17">
@@ -688,7 +688,7 @@
         <v>4C</v>
       </c>
       <c r="E17" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="18">
@@ -705,7 +705,7 @@
         <v>4E</v>
       </c>
       <c r="E18" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="19">
@@ -722,7 +722,7 @@
         <v>4G</v>
       </c>
       <c r="E19" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="20">
@@ -739,7 +739,7 @@
         <v>4I</v>
       </c>
       <c r="E20" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="21">
@@ -756,7 +756,7 @@
         <v>5B</v>
       </c>
       <c r="E21" t="str">
-        <v>John Doe5</v>
+        <v>John Doe0</v>
       </c>
     </row>
     <row r="22">
@@ -1113,7 +1113,7 @@
         <v>9G</v>
       </c>
       <c r="E42" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="43">
@@ -1130,7 +1130,7 @@
         <v>9I</v>
       </c>
       <c r="E43" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="44">
@@ -1147,7 +1147,7 @@
         <v>10A</v>
       </c>
       <c r="E44" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="45">
@@ -1164,7 +1164,7 @@
         <v>10C</v>
       </c>
       <c r="E45" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="46">
@@ -1181,7 +1181,7 @@
         <v>10E</v>
       </c>
       <c r="E46" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="47">
@@ -1198,7 +1198,7 @@
         <v>10G</v>
       </c>
       <c r="E47" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="48">
@@ -1215,7 +1215,7 @@
         <v>10I</v>
       </c>
       <c r="E48" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="49">
@@ -1232,7 +1232,7 @@
         <v>1A</v>
       </c>
       <c r="E49" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="50">
@@ -1249,7 +1249,7 @@
         <v>1C</v>
       </c>
       <c r="E50" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="51">
@@ -1266,7 +1266,7 @@
         <v>1E</v>
       </c>
       <c r="E51" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="52">
@@ -1283,7 +1283,7 @@
         <v>1G</v>
       </c>
       <c r="E52" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="53">
@@ -1300,7 +1300,7 @@
         <v>1I</v>
       </c>
       <c r="E53" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="54">
@@ -1317,7 +1317,7 @@
         <v>1K</v>
       </c>
       <c r="E54" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="55">
@@ -1334,7 +1334,7 @@
         <v>2B</v>
       </c>
       <c r="E55" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="56">
@@ -1351,7 +1351,7 @@
         <v>2D</v>
       </c>
       <c r="E56" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="57">
@@ -1368,7 +1368,7 @@
         <v>2F</v>
       </c>
       <c r="E57" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="58">
@@ -1385,7 +1385,7 @@
         <v>2H</v>
       </c>
       <c r="E58" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="59">
@@ -1402,7 +1402,7 @@
         <v>2J</v>
       </c>
       <c r="E59" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="60">
@@ -1419,7 +1419,7 @@
         <v>3C</v>
       </c>
       <c r="E60" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="61">
@@ -1436,7 +1436,7 @@
         <v>3E</v>
       </c>
       <c r="E61" t="str">
-        <v>John Doe5</v>
+        <v>John Doe10</v>
       </c>
     </row>
     <row r="62">
@@ -1453,7 +1453,7 @@
         <v>3G</v>
       </c>
       <c r="E62" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="63">
@@ -1470,7 +1470,7 @@
         <v>3I</v>
       </c>
       <c r="E63" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="64">
@@ -1487,7 +1487,7 @@
         <v>3K</v>
       </c>
       <c r="E64" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="65">
@@ -1504,7 +1504,7 @@
         <v>4A</v>
       </c>
       <c r="E65" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="66">
@@ -1521,7 +1521,7 @@
         <v>4C</v>
       </c>
       <c r="E66" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="67">
@@ -1538,7 +1538,7 @@
         <v>4E</v>
       </c>
       <c r="E67" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="68">
@@ -1555,7 +1555,7 @@
         <v>4G</v>
       </c>
       <c r="E68" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="69">
@@ -1572,7 +1572,7 @@
         <v>4I</v>
       </c>
       <c r="E69" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="70">
@@ -1589,7 +1589,7 @@
         <v>4K</v>
       </c>
       <c r="E70" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="71">
@@ -1606,7 +1606,7 @@
         <v>5B</v>
       </c>
       <c r="E71" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="72">
@@ -1623,7 +1623,7 @@
         <v>5D</v>
       </c>
       <c r="E72" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="73">
@@ -1640,7 +1640,7 @@
         <v>5F</v>
       </c>
       <c r="E73" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="74">
@@ -1657,7 +1657,7 @@
         <v>5H</v>
       </c>
       <c r="E74" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="75">
@@ -1674,7 +1674,7 @@
         <v>5J</v>
       </c>
       <c r="E75" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="76">
@@ -1691,7 +1691,7 @@
         <v>6C</v>
       </c>
       <c r="E76" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="77">
@@ -1708,7 +1708,7 @@
         <v>6E</v>
       </c>
       <c r="E77" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="78">
@@ -1725,7 +1725,7 @@
         <v>6G</v>
       </c>
       <c r="E78" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="79">
@@ -1742,7 +1742,7 @@
         <v>6I</v>
       </c>
       <c r="E79" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="80">
@@ -1759,7 +1759,7 @@
         <v>6K</v>
       </c>
       <c r="E80" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="81">
@@ -1776,7 +1776,7 @@
         <v>7A</v>
       </c>
       <c r="E81" t="str">
-        <v>John Doe5</v>
+        <v>John Doe15</v>
       </c>
     </row>
     <row r="82">
@@ -1793,7 +1793,7 @@
         <v>7C</v>
       </c>
       <c r="E82" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="83">
@@ -1810,7 +1810,7 @@
         <v>7E</v>
       </c>
       <c r="E83" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="84">
@@ -1827,7 +1827,7 @@
         <v>7G</v>
       </c>
       <c r="E84" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="85">
@@ -1844,7 +1844,7 @@
         <v>7I</v>
       </c>
       <c r="E85" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="86">
@@ -1861,7 +1861,7 @@
         <v>7K</v>
       </c>
       <c r="E86" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="87">
@@ -1878,7 +1878,7 @@
         <v>8B</v>
       </c>
       <c r="E87" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="88">
@@ -1895,7 +1895,7 @@
         <v>8D</v>
       </c>
       <c r="E88" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="89">
@@ -1912,7 +1912,7 @@
         <v>8F</v>
       </c>
       <c r="E89" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="90">
@@ -1929,7 +1929,7 @@
         <v>8H</v>
       </c>
       <c r="E90" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="91">
@@ -1946,7 +1946,7 @@
         <v>8J</v>
       </c>
       <c r="E91" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="92">
@@ -1963,7 +1963,7 @@
         <v>9C</v>
       </c>
       <c r="E92" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="93">
@@ -1980,7 +1980,7 @@
         <v>9E</v>
       </c>
       <c r="E93" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="94">
@@ -1997,7 +1997,7 @@
         <v>9G</v>
       </c>
       <c r="E94" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="95">
@@ -2014,7 +2014,7 @@
         <v>9I</v>
       </c>
       <c r="E95" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="96">
@@ -2031,7 +2031,7 @@
         <v>9K</v>
       </c>
       <c r="E96" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="97">
@@ -2048,7 +2048,7 @@
         <v>10A</v>
       </c>
       <c r="E97" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="98">
@@ -2065,7 +2065,7 @@
         <v>10C</v>
       </c>
       <c r="E98" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="99">
@@ -2082,7 +2082,7 @@
         <v>10E</v>
       </c>
       <c r="E99" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="100">
@@ -2099,7 +2099,7 @@
         <v>10G</v>
       </c>
       <c r="E100" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="101">
@@ -2116,7 +2116,7 @@
         <v>10I</v>
       </c>
       <c r="E101" t="str">
-        <v>John Doe5</v>
+        <v>John Doe20</v>
       </c>
     </row>
     <row r="102">
@@ -2133,7 +2133,7 @@
         <v>10K</v>
       </c>
       <c r="E102" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="103">
@@ -2150,7 +2150,7 @@
         <v>1A</v>
       </c>
       <c r="E103" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="104">
@@ -2167,7 +2167,7 @@
         <v>1C</v>
       </c>
       <c r="E104" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="105">
@@ -2184,7 +2184,7 @@
         <v>1E</v>
       </c>
       <c r="E105" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="106">
@@ -2201,7 +2201,7 @@
         <v>1G</v>
       </c>
       <c r="E106" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="107">
@@ -2218,7 +2218,7 @@
         <v>1I</v>
       </c>
       <c r="E107" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="108">
@@ -2235,7 +2235,7 @@
         <v>1K</v>
       </c>
       <c r="E108" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="109">
@@ -2252,7 +2252,7 @@
         <v>2B</v>
       </c>
       <c r="E109" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="110">
@@ -2269,7 +2269,7 @@
         <v>2D</v>
       </c>
       <c r="E110" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="111">
@@ -2286,7 +2286,7 @@
         <v>2F</v>
       </c>
       <c r="E111" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="112">
@@ -2303,7 +2303,7 @@
         <v>2H</v>
       </c>
       <c r="E112" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="113">
@@ -2320,7 +2320,7 @@
         <v>2J</v>
       </c>
       <c r="E113" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="114">
@@ -2337,7 +2337,7 @@
         <v>2L</v>
       </c>
       <c r="E114" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="115">
@@ -2354,7 +2354,7 @@
         <v>3C</v>
       </c>
       <c r="E115" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="116">
@@ -2371,7 +2371,7 @@
         <v>3E</v>
       </c>
       <c r="E116" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="117">
@@ -2388,7 +2388,7 @@
         <v>3G</v>
       </c>
       <c r="E117" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="118">
@@ -2405,7 +2405,7 @@
         <v>3I</v>
       </c>
       <c r="E118" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="119">
@@ -2422,7 +2422,7 @@
         <v>3K</v>
       </c>
       <c r="E119" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="120">
@@ -2439,7 +2439,7 @@
         <v>4A</v>
       </c>
       <c r="E120" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="121">
@@ -2456,7 +2456,7 @@
         <v>4C</v>
       </c>
       <c r="E121" t="str">
-        <v>John Doe5</v>
+        <v>John Doe25</v>
       </c>
     </row>
     <row r="122">
@@ -2473,7 +2473,7 @@
         <v>4E</v>
       </c>
       <c r="E122" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="123">
@@ -2490,7 +2490,7 @@
         <v>4G</v>
       </c>
       <c r="E123" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="124">
@@ -2507,7 +2507,7 @@
         <v>4I</v>
       </c>
       <c r="E124" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="125">
@@ -2524,7 +2524,7 @@
         <v>4K</v>
       </c>
       <c r="E125" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="126">
@@ -2541,7 +2541,7 @@
         <v>5B</v>
       </c>
       <c r="E126" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="127">
@@ -2558,7 +2558,7 @@
         <v>5D</v>
       </c>
       <c r="E127" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="128">
@@ -2575,7 +2575,7 @@
         <v>5F</v>
       </c>
       <c r="E128" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="129">
@@ -2592,7 +2592,7 @@
         <v>5H</v>
       </c>
       <c r="E129" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="130">
@@ -2609,7 +2609,7 @@
         <v>5J</v>
       </c>
       <c r="E130" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="131">
@@ -2626,7 +2626,7 @@
         <v>5L</v>
       </c>
       <c r="E131" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="132">
@@ -2643,7 +2643,7 @@
         <v>6C</v>
       </c>
       <c r="E132" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="133">
@@ -2660,7 +2660,7 @@
         <v>6E</v>
       </c>
       <c r="E133" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="134">
@@ -2677,7 +2677,7 @@
         <v>6G</v>
       </c>
       <c r="E134" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="135">
@@ -2694,7 +2694,7 @@
         <v>6I</v>
       </c>
       <c r="E135" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="136">
@@ -2711,7 +2711,7 @@
         <v>6K</v>
       </c>
       <c r="E136" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="137">
@@ -2728,7 +2728,7 @@
         <v>7A</v>
       </c>
       <c r="E137" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="138">
@@ -2745,7 +2745,7 @@
         <v>7C</v>
       </c>
       <c r="E138" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="139">
@@ -2762,7 +2762,7 @@
         <v>7E</v>
       </c>
       <c r="E139" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="140">
@@ -2779,7 +2779,7 @@
         <v>7G</v>
       </c>
       <c r="E140" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="141">
@@ -2796,7 +2796,7 @@
         <v>7I</v>
       </c>
       <c r="E141" t="str">
-        <v>John Doe5</v>
+        <v>John Doe30</v>
       </c>
     </row>
     <row r="142">
@@ -2813,7 +2813,7 @@
         <v>7K</v>
       </c>
       <c r="E142" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="143">
@@ -2830,7 +2830,7 @@
         <v>8B</v>
       </c>
       <c r="E143" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="144">
@@ -2847,7 +2847,7 @@
         <v>8D</v>
       </c>
       <c r="E144" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="145">
@@ -2864,7 +2864,7 @@
         <v>8F</v>
       </c>
       <c r="E145" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="146">
@@ -2881,7 +2881,7 @@
         <v>8H</v>
       </c>
       <c r="E146" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="147">
@@ -2898,7 +2898,7 @@
         <v>8J</v>
       </c>
       <c r="E147" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="148">
@@ -2915,7 +2915,7 @@
         <v>8L</v>
       </c>
       <c r="E148" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="149">
@@ -2932,7 +2932,7 @@
         <v>9C</v>
       </c>
       <c r="E149" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="150">
@@ -2949,7 +2949,7 @@
         <v>9E</v>
       </c>
       <c r="E150" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="151">
@@ -2966,7 +2966,7 @@
         <v>9G</v>
       </c>
       <c r="E151" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="152">
@@ -2983,7 +2983,7 @@
         <v>9I</v>
       </c>
       <c r="E152" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="153">
@@ -3000,7 +3000,7 @@
         <v>9K</v>
       </c>
       <c r="E153" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="154">
@@ -3017,7 +3017,7 @@
         <v>10A</v>
       </c>
       <c r="E154" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="155">
@@ -3034,7 +3034,7 @@
         <v>10C</v>
       </c>
       <c r="E155" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="156">
@@ -3051,7 +3051,7 @@
         <v>10E</v>
       </c>
       <c r="E156" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="157">
@@ -3068,7 +3068,7 @@
         <v>10G</v>
       </c>
       <c r="E157" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="158">
@@ -3085,7 +3085,7 @@
         <v>10I</v>
       </c>
       <c r="E158" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="159">
@@ -3102,7 +3102,7 @@
         <v>10K</v>
       </c>
       <c r="E159" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="160">
@@ -3119,7 +3119,7 @@
         <v>1A</v>
       </c>
       <c r="E160" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="161">
@@ -3136,7 +3136,7 @@
         <v>1C</v>
       </c>
       <c r="E161" t="str">
-        <v>John Doe5</v>
+        <v>John Doe35</v>
       </c>
     </row>
     <row r="162">
@@ -3153,7 +3153,7 @@
         <v>1E</v>
       </c>
       <c r="E162" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="163">
@@ -3170,7 +3170,7 @@
         <v>1G</v>
       </c>
       <c r="E163" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="164">
@@ -3187,7 +3187,7 @@
         <v>1I</v>
       </c>
       <c r="E164" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="165">
@@ -3204,7 +3204,7 @@
         <v>1K</v>
       </c>
       <c r="E165" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="166">
@@ -3221,7 +3221,7 @@
         <v>1M</v>
       </c>
       <c r="E166" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="167">
@@ -3238,7 +3238,7 @@
         <v>2B</v>
       </c>
       <c r="E167" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="168">
@@ -3255,7 +3255,7 @@
         <v>2D</v>
       </c>
       <c r="E168" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="169">
@@ -3272,7 +3272,7 @@
         <v>2F</v>
       </c>
       <c r="E169" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="170">
@@ -3289,7 +3289,7 @@
         <v>2H</v>
       </c>
       <c r="E170" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="171">
@@ -3306,7 +3306,7 @@
         <v>2J</v>
       </c>
       <c r="E171" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="172">
@@ -3323,7 +3323,7 @@
         <v>2L</v>
       </c>
       <c r="E172" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="173">
@@ -3340,7 +3340,7 @@
         <v>3C</v>
       </c>
       <c r="E173" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="174">
@@ -3357,7 +3357,7 @@
         <v>3E</v>
       </c>
       <c r="E174" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="175">
@@ -3374,7 +3374,7 @@
         <v>3G</v>
       </c>
       <c r="E175" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="176">
@@ -3391,7 +3391,7 @@
         <v>3I</v>
       </c>
       <c r="E176" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="177">
@@ -3408,7 +3408,7 @@
         <v>3K</v>
       </c>
       <c r="E177" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="178">
@@ -3425,7 +3425,7 @@
         <v>3M</v>
       </c>
       <c r="E178" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="179">
@@ -3442,7 +3442,7 @@
         <v>4A</v>
       </c>
       <c r="E179" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="180">
@@ -3459,7 +3459,7 @@
         <v>4C</v>
       </c>
       <c r="E180" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="181">
@@ -3476,7 +3476,7 @@
         <v>4E</v>
       </c>
       <c r="E181" t="str">
-        <v>John Doe5</v>
+        <v>John Doe40</v>
       </c>
     </row>
     <row r="182">
@@ -3493,7 +3493,7 @@
         <v>4G</v>
       </c>
       <c r="E182" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="183">
@@ -3510,7 +3510,7 @@
         <v>4I</v>
       </c>
       <c r="E183" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="184">
@@ -3527,7 +3527,7 @@
         <v>4K</v>
       </c>
       <c r="E184" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="185">
@@ -3544,7 +3544,7 @@
         <v>4M</v>
       </c>
       <c r="E185" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="186">
@@ -3561,7 +3561,7 @@
         <v>5B</v>
       </c>
       <c r="E186" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="187">
@@ -3578,7 +3578,7 @@
         <v>5D</v>
       </c>
       <c r="E187" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="188">
@@ -3595,7 +3595,7 @@
         <v>5F</v>
       </c>
       <c r="E188" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="189">
@@ -3612,7 +3612,7 @@
         <v>5H</v>
       </c>
       <c r="E189" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="190">
@@ -3629,7 +3629,7 @@
         <v>5J</v>
       </c>
       <c r="E190" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="191">
@@ -3646,7 +3646,7 @@
         <v>5L</v>
       </c>
       <c r="E191" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="192">
@@ -3663,7 +3663,7 @@
         <v>6C</v>
       </c>
       <c r="E192" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="193">
@@ -3680,7 +3680,7 @@
         <v>6E</v>
       </c>
       <c r="E193" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="194">
@@ -3697,7 +3697,7 @@
         <v>6G</v>
       </c>
       <c r="E194" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="195">
@@ -3714,7 +3714,7 @@
         <v>6I</v>
       </c>
       <c r="E195" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="196">
@@ -3731,7 +3731,7 @@
         <v>6K</v>
       </c>
       <c r="E196" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="197">
@@ -3748,7 +3748,7 @@
         <v>6M</v>
       </c>
       <c r="E197" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="198">
@@ -3765,7 +3765,7 @@
         <v>7A</v>
       </c>
       <c r="E198" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="199">
@@ -3782,7 +3782,7 @@
         <v>7C</v>
       </c>
       <c r="E199" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="200">
@@ -3799,7 +3799,7 @@
         <v>7E</v>
       </c>
       <c r="E200" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="201">
@@ -3816,7 +3816,7 @@
         <v>7G</v>
       </c>
       <c r="E201" t="str">
-        <v>John Doe5</v>
+        <v>John Doe45</v>
       </c>
     </row>
     <row r="202">
@@ -3832,9 +3832,6 @@
       <c r="D202" t="str">
         <v>7I</v>
       </c>
-      <c r="E202" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203">
@@ -3849,9 +3846,6 @@
       <c r="D203" t="str">
         <v>7K</v>
       </c>
-      <c r="E203" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204">
@@ -3866,9 +3860,6 @@
       <c r="D204" t="str">
         <v>7M</v>
       </c>
-      <c r="E204" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205">
@@ -3883,9 +3874,6 @@
       <c r="D205" t="str">
         <v>8B</v>
       </c>
-      <c r="E205" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206">
@@ -3900,9 +3888,6 @@
       <c r="D206" t="str">
         <v>8D</v>
       </c>
-      <c r="E206" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207">
@@ -3917,9 +3902,6 @@
       <c r="D207" t="str">
         <v>8F</v>
       </c>
-      <c r="E207" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208">
@@ -3934,9 +3916,6 @@
       <c r="D208" t="str">
         <v>8H</v>
       </c>
-      <c r="E208" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209">
@@ -3951,9 +3930,6 @@
       <c r="D209" t="str">
         <v>8J</v>
       </c>
-      <c r="E209" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210">
@@ -3968,9 +3944,6 @@
       <c r="D210" t="str">
         <v>8L</v>
       </c>
-      <c r="E210" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211">
@@ -3985,9 +3958,6 @@
       <c r="D211" t="str">
         <v>9C</v>
       </c>
-      <c r="E211" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212">
@@ -4002,9 +3972,6 @@
       <c r="D212" t="str">
         <v>9E</v>
       </c>
-      <c r="E212" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213">
@@ -4019,9 +3986,6 @@
       <c r="D213" t="str">
         <v>9G</v>
       </c>
-      <c r="E213" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214">
@@ -4036,9 +4000,6 @@
       <c r="D214" t="str">
         <v>9I</v>
       </c>
-      <c r="E214" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215">
@@ -4053,9 +4014,6 @@
       <c r="D215" t="str">
         <v>9K</v>
       </c>
-      <c r="E215" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216">
@@ -4070,9 +4028,6 @@
       <c r="D216" t="str">
         <v>9M</v>
       </c>
-      <c r="E216" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217">
@@ -4087,9 +4042,6 @@
       <c r="D217" t="str">
         <v>10A</v>
       </c>
-      <c r="E217" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218">
@@ -4104,9 +4056,6 @@
       <c r="D218" t="str">
         <v>10C</v>
       </c>
-      <c r="E218" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219">
@@ -4121,9 +4070,6 @@
       <c r="D219" t="str">
         <v>10E</v>
       </c>
-      <c r="E219" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220">
@@ -4138,9 +4084,6 @@
       <c r="D220" t="str">
         <v>10G</v>
       </c>
-      <c r="E220" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221">
@@ -4155,9 +4098,6 @@
       <c r="D221" t="str">
         <v>10I</v>
       </c>
-      <c r="E221" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222">
@@ -4172,9 +4112,6 @@
       <c r="D222" t="str">
         <v>10K</v>
       </c>
-      <c r="E222" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223">
@@ -4189,9 +4126,6 @@
       <c r="D223" t="str">
         <v>10M</v>
       </c>
-      <c r="E223" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224">
@@ -4206,9 +4140,6 @@
       <c r="D224" t="str">
         <v>1A</v>
       </c>
-      <c r="E224" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225">
@@ -4223,9 +4154,6 @@
       <c r="D225" t="str">
         <v>1C</v>
       </c>
-      <c r="E225" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226">
@@ -4240,9 +4168,6 @@
       <c r="D226" t="str">
         <v>1E</v>
       </c>
-      <c r="E226" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227">
@@ -4257,9 +4182,6 @@
       <c r="D227" t="str">
         <v>1G</v>
       </c>
-      <c r="E227" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228">
@@ -4274,9 +4196,6 @@
       <c r="D228" t="str">
         <v>1I</v>
       </c>
-      <c r="E228" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229">
@@ -4291,9 +4210,6 @@
       <c r="D229" t="str">
         <v>1K</v>
       </c>
-      <c r="E229" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230">
@@ -4308,9 +4224,6 @@
       <c r="D230" t="str">
         <v>1M</v>
       </c>
-      <c r="E230" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231">
@@ -4325,9 +4238,6 @@
       <c r="D231" t="str">
         <v>2B</v>
       </c>
-      <c r="E231" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="232">
       <c r="A232">
@@ -4342,9 +4252,6 @@
       <c r="D232" t="str">
         <v>2D</v>
       </c>
-      <c r="E232" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233">
@@ -4359,9 +4266,6 @@
       <c r="D233" t="str">
         <v>2F</v>
       </c>
-      <c r="E233" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="234">
       <c r="A234">
@@ -4376,9 +4280,6 @@
       <c r="D234" t="str">
         <v>2H</v>
       </c>
-      <c r="E234" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235">
@@ -4393,9 +4294,6 @@
       <c r="D235" t="str">
         <v>2J</v>
       </c>
-      <c r="E235" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236">
@@ -4410,9 +4308,6 @@
       <c r="D236" t="str">
         <v>2L</v>
       </c>
-      <c r="E236" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237">
@@ -4427,9 +4322,6 @@
       <c r="D237" t="str">
         <v>2N</v>
       </c>
-      <c r="E237" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238">
@@ -4444,9 +4336,6 @@
       <c r="D238" t="str">
         <v>3C</v>
       </c>
-      <c r="E238" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239">
@@ -4461,9 +4350,6 @@
       <c r="D239" t="str">
         <v>3E</v>
       </c>
-      <c r="E239" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240">
@@ -4478,9 +4364,6 @@
       <c r="D240" t="str">
         <v>3G</v>
       </c>
-      <c r="E240" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241">
@@ -4495,9 +4378,6 @@
       <c r="D241" t="str">
         <v>3I</v>
       </c>
-      <c r="E241" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242">
@@ -4512,9 +4392,6 @@
       <c r="D242" t="str">
         <v>3K</v>
       </c>
-      <c r="E242" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243">
@@ -4529,9 +4406,6 @@
       <c r="D243" t="str">
         <v>3M</v>
       </c>
-      <c r="E243" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244">
@@ -4546,9 +4420,6 @@
       <c r="D244" t="str">
         <v>4A</v>
       </c>
-      <c r="E244" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245">
@@ -4563,9 +4434,6 @@
       <c r="D245" t="str">
         <v>4C</v>
       </c>
-      <c r="E245" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="246">
       <c r="A246">
@@ -4580,9 +4448,6 @@
       <c r="D246" t="str">
         <v>4E</v>
       </c>
-      <c r="E246" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247">
@@ -4597,9 +4462,6 @@
       <c r="D247" t="str">
         <v>4G</v>
       </c>
-      <c r="E247" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248">
@@ -4614,9 +4476,6 @@
       <c r="D248" t="str">
         <v>4I</v>
       </c>
-      <c r="E248" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="249">
       <c r="A249">
@@ -4631,9 +4490,6 @@
       <c r="D249" t="str">
         <v>4K</v>
       </c>
-      <c r="E249" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="250">
       <c r="A250">
@@ -4648,9 +4504,6 @@
       <c r="D250" t="str">
         <v>4M</v>
       </c>
-      <c r="E250" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="251">
       <c r="A251">
@@ -4665,9 +4518,6 @@
       <c r="D251" t="str">
         <v>5B</v>
       </c>
-      <c r="E251" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="252">
       <c r="A252">
@@ -4682,9 +4532,6 @@
       <c r="D252" t="str">
         <v>5D</v>
       </c>
-      <c r="E252" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="253">
       <c r="A253">
@@ -4699,9 +4546,6 @@
       <c r="D253" t="str">
         <v>5F</v>
       </c>
-      <c r="E253" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="254">
       <c r="A254">
@@ -4716,9 +4560,6 @@
       <c r="D254" t="str">
         <v>5H</v>
       </c>
-      <c r="E254" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="255">
       <c r="A255">
@@ -4733,9 +4574,6 @@
       <c r="D255" t="str">
         <v>5J</v>
       </c>
-      <c r="E255" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="256">
       <c r="A256">
@@ -4750,9 +4588,6 @@
       <c r="D256" t="str">
         <v>5L</v>
       </c>
-      <c r="E256" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="257">
       <c r="A257">
@@ -4767,9 +4602,6 @@
       <c r="D257" t="str">
         <v>5N</v>
       </c>
-      <c r="E257" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="258">
       <c r="A258">
@@ -4784,9 +4616,6 @@
       <c r="D258" t="str">
         <v>6C</v>
       </c>
-      <c r="E258" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="259">
       <c r="A259">
@@ -4801,9 +4630,6 @@
       <c r="D259" t="str">
         <v>6E</v>
       </c>
-      <c r="E259" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="260">
       <c r="A260">
@@ -4818,9 +4644,6 @@
       <c r="D260" t="str">
         <v>6G</v>
       </c>
-      <c r="E260" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="261">
       <c r="A261">
@@ -4835,9 +4658,6 @@
       <c r="D261" t="str">
         <v>6I</v>
       </c>
-      <c r="E261" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="262">
       <c r="A262">
@@ -4852,9 +4672,6 @@
       <c r="D262" t="str">
         <v>6K</v>
       </c>
-      <c r="E262" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="263">
       <c r="A263">
@@ -4869,9 +4686,6 @@
       <c r="D263" t="str">
         <v>6M</v>
       </c>
-      <c r="E263" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="264">
       <c r="A264">
@@ -4886,9 +4700,6 @@
       <c r="D264" t="str">
         <v>7A</v>
       </c>
-      <c r="E264" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="265">
       <c r="A265">
@@ -4903,9 +4714,6 @@
       <c r="D265" t="str">
         <v>7C</v>
       </c>
-      <c r="E265" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="266">
       <c r="A266">
@@ -4920,9 +4728,6 @@
       <c r="D266" t="str">
         <v>7E</v>
       </c>
-      <c r="E266" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="267">
       <c r="A267">
@@ -4937,9 +4742,6 @@
       <c r="D267" t="str">
         <v>7G</v>
       </c>
-      <c r="E267" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="268">
       <c r="A268">
@@ -4954,9 +4756,6 @@
       <c r="D268" t="str">
         <v>7I</v>
       </c>
-      <c r="E268" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="269">
       <c r="A269">
@@ -4971,9 +4770,6 @@
       <c r="D269" t="str">
         <v>7K</v>
       </c>
-      <c r="E269" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="270">
       <c r="A270">
@@ -4988,9 +4784,6 @@
       <c r="D270" t="str">
         <v>7M</v>
       </c>
-      <c r="E270" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="271">
       <c r="A271">
@@ -5005,9 +4798,6 @@
       <c r="D271" t="str">
         <v>8B</v>
       </c>
-      <c r="E271" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="272">
       <c r="A272">
@@ -5022,9 +4812,6 @@
       <c r="D272" t="str">
         <v>8D</v>
       </c>
-      <c r="E272" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="273">
       <c r="A273">
@@ -5039,9 +4826,6 @@
       <c r="D273" t="str">
         <v>8F</v>
       </c>
-      <c r="E273" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="274">
       <c r="A274">
@@ -5056,9 +4840,6 @@
       <c r="D274" t="str">
         <v>8H</v>
       </c>
-      <c r="E274" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="275">
       <c r="A275">
@@ -5073,9 +4854,6 @@
       <c r="D275" t="str">
         <v>8J</v>
       </c>
-      <c r="E275" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="276">
       <c r="A276">
@@ -5090,9 +4868,6 @@
       <c r="D276" t="str">
         <v>8L</v>
       </c>
-      <c r="E276" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="277">
       <c r="A277">
@@ -5107,9 +4882,6 @@
       <c r="D277" t="str">
         <v>8N</v>
       </c>
-      <c r="E277" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="278">
       <c r="A278">
@@ -5124,9 +4896,6 @@
       <c r="D278" t="str">
         <v>9C</v>
       </c>
-      <c r="E278" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="279">
       <c r="A279">
@@ -5141,9 +4910,6 @@
       <c r="D279" t="str">
         <v>9E</v>
       </c>
-      <c r="E279" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="280">
       <c r="A280">
@@ -5158,9 +4924,6 @@
       <c r="D280" t="str">
         <v>9G</v>
       </c>
-      <c r="E280" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="281">
       <c r="A281">
@@ -5175,9 +4938,6 @@
       <c r="D281" t="str">
         <v>9I</v>
       </c>
-      <c r="E281" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="282">
       <c r="A282">
@@ -5192,9 +4952,6 @@
       <c r="D282" t="str">
         <v>9K</v>
       </c>
-      <c r="E282" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="283">
       <c r="A283">
@@ -5209,9 +4966,6 @@
       <c r="D283" t="str">
         <v>9M</v>
       </c>
-      <c r="E283" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="284">
       <c r="A284">
@@ -5226,9 +4980,6 @@
       <c r="D284" t="str">
         <v>10A</v>
       </c>
-      <c r="E284" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="285">
       <c r="A285">
@@ -5243,9 +4994,6 @@
       <c r="D285" t="str">
         <v>10C</v>
       </c>
-      <c r="E285" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="286">
       <c r="A286">
@@ -5260,9 +5008,6 @@
       <c r="D286" t="str">
         <v>10E</v>
       </c>
-      <c r="E286" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="287">
       <c r="A287">
@@ -5277,9 +5022,6 @@
       <c r="D287" t="str">
         <v>10G</v>
       </c>
-      <c r="E287" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="288">
       <c r="A288">
@@ -5294,9 +5036,6 @@
       <c r="D288" t="str">
         <v>10I</v>
       </c>
-      <c r="E288" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="289">
       <c r="A289">
@@ -5311,9 +5050,6 @@
       <c r="D289" t="str">
         <v>10K</v>
       </c>
-      <c r="E289" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="290">
       <c r="A290">
@@ -5328,9 +5064,6 @@
       <c r="D290" t="str">
         <v>10M</v>
       </c>
-      <c r="E290" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="291">
       <c r="A291">
@@ -5345,9 +5078,6 @@
       <c r="D291" t="str">
         <v>1A</v>
       </c>
-      <c r="E291" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="292">
       <c r="A292">
@@ -5362,9 +5092,6 @@
       <c r="D292" t="str">
         <v>1C</v>
       </c>
-      <c r="E292" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="293">
       <c r="A293">
@@ -5379,9 +5106,6 @@
       <c r="D293" t="str">
         <v>1E</v>
       </c>
-      <c r="E293" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="294">
       <c r="A294">
@@ -5396,9 +5120,6 @@
       <c r="D294" t="str">
         <v>1G</v>
       </c>
-      <c r="E294" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="295">
       <c r="A295">
@@ -5413,9 +5134,6 @@
       <c r="D295" t="str">
         <v>1I</v>
       </c>
-      <c r="E295" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="296">
       <c r="A296">
@@ -5430,9 +5148,6 @@
       <c r="D296" t="str">
         <v>1K</v>
       </c>
-      <c r="E296" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="297">
       <c r="A297">
@@ -5447,9 +5162,6 @@
       <c r="D297" t="str">
         <v>1M</v>
       </c>
-      <c r="E297" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="298">
       <c r="A298">
@@ -5464,9 +5176,6 @@
       <c r="D298" t="str">
         <v>1O</v>
       </c>
-      <c r="E298" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="299">
       <c r="A299">
@@ -5481,9 +5190,6 @@
       <c r="D299" t="str">
         <v>2B</v>
       </c>
-      <c r="E299" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="300">
       <c r="A300">
@@ -5498,9 +5204,6 @@
       <c r="D300" t="str">
         <v>2D</v>
       </c>
-      <c r="E300" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="301">
       <c r="A301">
@@ -5515,9 +5218,6 @@
       <c r="D301" t="str">
         <v>2F</v>
       </c>
-      <c r="E301" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="302">
       <c r="A302">
@@ -5532,9 +5232,6 @@
       <c r="D302" t="str">
         <v>2H</v>
       </c>
-      <c r="E302" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="303">
       <c r="A303">
@@ -5549,9 +5246,6 @@
       <c r="D303" t="str">
         <v>2J</v>
       </c>
-      <c r="E303" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="304">
       <c r="A304">
@@ -5566,9 +5260,6 @@
       <c r="D304" t="str">
         <v>2L</v>
       </c>
-      <c r="E304" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="305">
       <c r="A305">
@@ -5583,9 +5274,6 @@
       <c r="D305" t="str">
         <v>2N</v>
       </c>
-      <c r="E305" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="306">
       <c r="A306">
@@ -5600,9 +5288,6 @@
       <c r="D306" t="str">
         <v>3C</v>
       </c>
-      <c r="E306" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="307">
       <c r="A307">
@@ -5617,9 +5302,6 @@
       <c r="D307" t="str">
         <v>3E</v>
       </c>
-      <c r="E307" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="308">
       <c r="A308">
@@ -5634,9 +5316,6 @@
       <c r="D308" t="str">
         <v>3G</v>
       </c>
-      <c r="E308" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="309">
       <c r="A309">
@@ -5651,9 +5330,6 @@
       <c r="D309" t="str">
         <v>3I</v>
       </c>
-      <c r="E309" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="310">
       <c r="A310">
@@ -5668,9 +5344,6 @@
       <c r="D310" t="str">
         <v>3K</v>
       </c>
-      <c r="E310" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="311">
       <c r="A311">
@@ -5685,9 +5358,6 @@
       <c r="D311" t="str">
         <v>3M</v>
       </c>
-      <c r="E311" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="312">
       <c r="A312">
@@ -5702,9 +5372,6 @@
       <c r="D312" t="str">
         <v>3O</v>
       </c>
-      <c r="E312" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="313">
       <c r="A313">
@@ -5719,9 +5386,6 @@
       <c r="D313" t="str">
         <v>4A</v>
       </c>
-      <c r="E313" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="314">
       <c r="A314">
@@ -5736,9 +5400,6 @@
       <c r="D314" t="str">
         <v>4C</v>
       </c>
-      <c r="E314" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="315">
       <c r="A315">
@@ -5753,9 +5414,6 @@
       <c r="D315" t="str">
         <v>4E</v>
       </c>
-      <c r="E315" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="316">
       <c r="A316">
@@ -5770,9 +5428,6 @@
       <c r="D316" t="str">
         <v>4G</v>
       </c>
-      <c r="E316" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="317">
       <c r="A317">
@@ -5787,9 +5442,6 @@
       <c r="D317" t="str">
         <v>4I</v>
       </c>
-      <c r="E317" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="318">
       <c r="A318">
@@ -5804,9 +5456,6 @@
       <c r="D318" t="str">
         <v>4K</v>
       </c>
-      <c r="E318" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="319">
       <c r="A319">
@@ -5821,9 +5470,6 @@
       <c r="D319" t="str">
         <v>4M</v>
       </c>
-      <c r="E319" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="320">
       <c r="A320">
@@ -5838,9 +5484,6 @@
       <c r="D320" t="str">
         <v>4O</v>
       </c>
-      <c r="E320" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="321">
       <c r="A321">
@@ -5855,9 +5498,6 @@
       <c r="D321" t="str">
         <v>5B</v>
       </c>
-      <c r="E321" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="322">
       <c r="A322">
@@ -5872,9 +5512,6 @@
       <c r="D322" t="str">
         <v>5D</v>
       </c>
-      <c r="E322" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="323">
       <c r="A323">
@@ -5889,9 +5526,6 @@
       <c r="D323" t="str">
         <v>5F</v>
       </c>
-      <c r="E323" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="324">
       <c r="A324">
@@ -5906,9 +5540,6 @@
       <c r="D324" t="str">
         <v>5H</v>
       </c>
-      <c r="E324" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="325">
       <c r="A325">
@@ -5923,9 +5554,6 @@
       <c r="D325" t="str">
         <v>5J</v>
       </c>
-      <c r="E325" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="326">
       <c r="A326">
@@ -5940,9 +5568,6 @@
       <c r="D326" t="str">
         <v>5L</v>
       </c>
-      <c r="E326" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="327">
       <c r="A327">
@@ -5957,9 +5582,6 @@
       <c r="D327" t="str">
         <v>5N</v>
       </c>
-      <c r="E327" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="328">
       <c r="A328">
@@ -5974,9 +5596,6 @@
       <c r="D328" t="str">
         <v>6C</v>
       </c>
-      <c r="E328" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="329">
       <c r="A329">
@@ -5991,9 +5610,6 @@
       <c r="D329" t="str">
         <v>6E</v>
       </c>
-      <c r="E329" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="330">
       <c r="A330">
@@ -6008,9 +5624,6 @@
       <c r="D330" t="str">
         <v>6G</v>
       </c>
-      <c r="E330" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="331">
       <c r="A331">
@@ -6025,9 +5638,6 @@
       <c r="D331" t="str">
         <v>6I</v>
       </c>
-      <c r="E331" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="332">
       <c r="A332">
@@ -6042,9 +5652,6 @@
       <c r="D332" t="str">
         <v>6K</v>
       </c>
-      <c r="E332" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="333">
       <c r="A333">
@@ -6059,9 +5666,6 @@
       <c r="D333" t="str">
         <v>6M</v>
       </c>
-      <c r="E333" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="334">
       <c r="A334">
@@ -6076,9 +5680,6 @@
       <c r="D334" t="str">
         <v>6O</v>
       </c>
-      <c r="E334" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="335">
       <c r="A335">
@@ -6093,9 +5694,6 @@
       <c r="D335" t="str">
         <v>7A</v>
       </c>
-      <c r="E335" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="336">
       <c r="A336">
@@ -6110,9 +5708,6 @@
       <c r="D336" t="str">
         <v>7C</v>
       </c>
-      <c r="E336" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="337">
       <c r="A337">
@@ -6127,9 +5722,6 @@
       <c r="D337" t="str">
         <v>7E</v>
       </c>
-      <c r="E337" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="338">
       <c r="A338">
@@ -6144,9 +5736,6 @@
       <c r="D338" t="str">
         <v>7G</v>
       </c>
-      <c r="E338" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="339">
       <c r="A339">
@@ -6161,9 +5750,6 @@
       <c r="D339" t="str">
         <v>7I</v>
       </c>
-      <c r="E339" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="340">
       <c r="A340">
@@ -6178,9 +5764,6 @@
       <c r="D340" t="str">
         <v>7K</v>
       </c>
-      <c r="E340" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="341">
       <c r="A341">
@@ -6195,9 +5778,6 @@
       <c r="D341" t="str">
         <v>7M</v>
       </c>
-      <c r="E341" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="342">
       <c r="A342">
@@ -6212,9 +5792,6 @@
       <c r="D342" t="str">
         <v>7O</v>
       </c>
-      <c r="E342" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="343">
       <c r="A343">
@@ -6229,9 +5806,6 @@
       <c r="D343" t="str">
         <v>8B</v>
       </c>
-      <c r="E343" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="344">
       <c r="A344">
@@ -6246,9 +5820,6 @@
       <c r="D344" t="str">
         <v>8D</v>
       </c>
-      <c r="E344" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="345">
       <c r="A345">
@@ -6263,9 +5834,6 @@
       <c r="D345" t="str">
         <v>8F</v>
       </c>
-      <c r="E345" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="346">
       <c r="A346">
@@ -6280,9 +5848,6 @@
       <c r="D346" t="str">
         <v>8H</v>
       </c>
-      <c r="E346" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="347">
       <c r="A347">
@@ -6297,9 +5862,6 @@
       <c r="D347" t="str">
         <v>8J</v>
       </c>
-      <c r="E347" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="348">
       <c r="A348">
@@ -6314,9 +5876,6 @@
       <c r="D348" t="str">
         <v>8L</v>
       </c>
-      <c r="E348" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="349">
       <c r="A349">
@@ -6331,9 +5890,6 @@
       <c r="D349" t="str">
         <v>8N</v>
       </c>
-      <c r="E349" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="350">
       <c r="A350">
@@ -6348,9 +5904,6 @@
       <c r="D350" t="str">
         <v>9C</v>
       </c>
-      <c r="E350" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="351">
       <c r="A351">
@@ -6365,9 +5918,6 @@
       <c r="D351" t="str">
         <v>9E</v>
       </c>
-      <c r="E351" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="352">
       <c r="A352">
@@ -6382,9 +5932,6 @@
       <c r="D352" t="str">
         <v>9G</v>
       </c>
-      <c r="E352" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="353">
       <c r="A353">
@@ -6399,9 +5946,6 @@
       <c r="D353" t="str">
         <v>9I</v>
       </c>
-      <c r="E353" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="354">
       <c r="A354">
@@ -6416,9 +5960,6 @@
       <c r="D354" t="str">
         <v>9K</v>
       </c>
-      <c r="E354" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="355">
       <c r="A355">
@@ -6433,9 +5974,6 @@
       <c r="D355" t="str">
         <v>9M</v>
       </c>
-      <c r="E355" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="356">
       <c r="A356">
@@ -6450,9 +5988,6 @@
       <c r="D356" t="str">
         <v>9O</v>
       </c>
-      <c r="E356" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="357">
       <c r="A357">
@@ -6467,9 +6002,6 @@
       <c r="D357" t="str">
         <v>10A</v>
       </c>
-      <c r="E357" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="358">
       <c r="A358">
@@ -6484,9 +6016,6 @@
       <c r="D358" t="str">
         <v>10C</v>
       </c>
-      <c r="E358" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="359">
       <c r="A359">
@@ -6501,9 +6030,6 @@
       <c r="D359" t="str">
         <v>10E</v>
       </c>
-      <c r="E359" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="360">
       <c r="A360">
@@ -6518,9 +6044,6 @@
       <c r="D360" t="str">
         <v>10G</v>
       </c>
-      <c r="E360" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="361">
       <c r="A361">
@@ -6535,9 +6058,6 @@
       <c r="D361" t="str">
         <v>10I</v>
       </c>
-      <c r="E361" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="362">
       <c r="A362">
@@ -6552,9 +6072,6 @@
       <c r="D362" t="str">
         <v>10K</v>
       </c>
-      <c r="E362" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="363">
       <c r="A363">
@@ -6569,9 +6086,6 @@
       <c r="D363" t="str">
         <v>10M</v>
       </c>
-      <c r="E363" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="364">
       <c r="A364">
@@ -6586,9 +6100,6 @@
       <c r="D364" t="str">
         <v>10O</v>
       </c>
-      <c r="E364" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="365">
       <c r="A365">
@@ -6603,9 +6114,6 @@
       <c r="D365" t="str">
         <v>1A</v>
       </c>
-      <c r="E365" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="366">
       <c r="A366">
@@ -6620,9 +6128,6 @@
       <c r="D366" t="str">
         <v>1C</v>
       </c>
-      <c r="E366" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="367">
       <c r="A367">
@@ -6637,9 +6142,6 @@
       <c r="D367" t="str">
         <v>1E</v>
       </c>
-      <c r="E367" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="368">
       <c r="A368">
@@ -6654,9 +6156,6 @@
       <c r="D368" t="str">
         <v>1G</v>
       </c>
-      <c r="E368" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="369">
       <c r="A369">
@@ -6671,9 +6170,6 @@
       <c r="D369" t="str">
         <v>1I</v>
       </c>
-      <c r="E369" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="370">
       <c r="A370">
@@ -6688,9 +6184,6 @@
       <c r="D370" t="str">
         <v>1K</v>
       </c>
-      <c r="E370" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="371">
       <c r="A371">
@@ -6705,9 +6198,6 @@
       <c r="D371" t="str">
         <v>1M</v>
       </c>
-      <c r="E371" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="372">
       <c r="A372">
@@ -6722,9 +6212,6 @@
       <c r="D372" t="str">
         <v>1O</v>
       </c>
-      <c r="E372" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="373">
       <c r="A373">
@@ -6739,9 +6226,6 @@
       <c r="D373" t="str">
         <v>2B</v>
       </c>
-      <c r="E373" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="374">
       <c r="A374">
@@ -6756,9 +6240,6 @@
       <c r="D374" t="str">
         <v>2D</v>
       </c>
-      <c r="E374" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="375">
       <c r="A375">
@@ -6773,9 +6254,6 @@
       <c r="D375" t="str">
         <v>2F</v>
       </c>
-      <c r="E375" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="376">
       <c r="A376">
@@ -6790,9 +6268,6 @@
       <c r="D376" t="str">
         <v>2H</v>
       </c>
-      <c r="E376" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="377">
       <c r="A377">
@@ -6807,9 +6282,6 @@
       <c r="D377" t="str">
         <v>2J</v>
       </c>
-      <c r="E377" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="378">
       <c r="A378">
@@ -6824,9 +6296,6 @@
       <c r="D378" t="str">
         <v>2L</v>
       </c>
-      <c r="E378" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="379">
       <c r="A379">
@@ -6841,9 +6310,6 @@
       <c r="D379" t="str">
         <v>2N</v>
       </c>
-      <c r="E379" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="380">
       <c r="A380">
@@ -6858,9 +6324,6 @@
       <c r="D380" t="str">
         <v>2P</v>
       </c>
-      <c r="E380" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="381">
       <c r="A381">
@@ -6875,9 +6338,6 @@
       <c r="D381" t="str">
         <v>3C</v>
       </c>
-      <c r="E381" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="382">
       <c r="A382">
@@ -6892,9 +6352,6 @@
       <c r="D382" t="str">
         <v>3E</v>
       </c>
-      <c r="E382" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="383">
       <c r="A383">
@@ -6909,9 +6366,6 @@
       <c r="D383" t="str">
         <v>3G</v>
       </c>
-      <c r="E383" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="384">
       <c r="A384">
@@ -6926,9 +6380,6 @@
       <c r="D384" t="str">
         <v>3I</v>
       </c>
-      <c r="E384" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="385">
       <c r="A385">
@@ -6943,9 +6394,6 @@
       <c r="D385" t="str">
         <v>3K</v>
       </c>
-      <c r="E385" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="386">
       <c r="A386">
@@ -6960,9 +6408,6 @@
       <c r="D386" t="str">
         <v>3M</v>
       </c>
-      <c r="E386" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="387">
       <c r="A387">
@@ -6977,9 +6422,6 @@
       <c r="D387" t="str">
         <v>3O</v>
       </c>
-      <c r="E387" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="388">
       <c r="A388">
@@ -6994,9 +6436,6 @@
       <c r="D388" t="str">
         <v>4A</v>
       </c>
-      <c r="E388" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="389">
       <c r="A389">
@@ -7011,9 +6450,6 @@
       <c r="D389" t="str">
         <v>4C</v>
       </c>
-      <c r="E389" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="390">
       <c r="A390">
@@ -7028,9 +6464,6 @@
       <c r="D390" t="str">
         <v>4E</v>
       </c>
-      <c r="E390" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="391">
       <c r="A391">
@@ -7045,9 +6478,6 @@
       <c r="D391" t="str">
         <v>4G</v>
       </c>
-      <c r="E391" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="392">
       <c r="A392">
@@ -7062,9 +6492,6 @@
       <c r="D392" t="str">
         <v>4I</v>
       </c>
-      <c r="E392" t="str">
-        <v>John Doe5</v>
-      </c>
     </row>
     <row r="393">
       <c r="A393">
@@ -7078,9 +6505,6 @@
       </c>
       <c r="D393" t="str">
         <v>4K</v>
-      </c>
-      <c r="E393" t="str">
-        <v>John Doe5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>